<commit_message>
corect the shrinkage in th moo.morphology and run again for 1.0 1.0
</commit_message>
<xml_diff>
--- a/cells_initial_information/Data2.xlsx
+++ b/cells_initial_information/Data2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t xml:space="preserve">cell_name</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t xml:space="preserve">mouse_spine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neck </t>
   </si>
   <si>
     <t xml:space="preserve">shaft_spine</t>
@@ -888,7 +891,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1390,8 +1393,8 @@
   </sheetPr>
   <dimension ref="A1:AY40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3032,8 +3035,8 @@
       <c r="R18" s="41"/>
       <c r="S18" s="41"/>
       <c r="T18" s="41"/>
-      <c r="U18" s="131" t="n">
-        <v>0.37</v>
+      <c r="U18" s="131" t="s">
+        <v>60</v>
       </c>
       <c r="V18" s="72" t="n">
         <v>1.08</v>
@@ -3047,7 +3050,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="134" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" s="135"/>
       <c r="C19" s="46"/>
@@ -3094,7 +3097,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="138" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B20" s="139"/>
       <c r="C20" s="140"/>

</xml_diff>

<commit_message>
all th edata groger sent m etogete=her
</commit_message>
<xml_diff>
--- a/cells_initial_information/Data2.xlsx
+++ b/cells_initial_information/Data2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t xml:space="preserve">cell_name</t>
   </si>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t xml:space="preserve">mouse_spine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">neck </t>
   </si>
   <si>
     <t xml:space="preserve">shaft_spine</t>
@@ -225,6 +222,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -246,6 +244,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -253,12 +252,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -266,6 +267,7 @@
       <color rgb="FF81D41A"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -273,6 +275,7 @@
       <color rgb="FFFF972F"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -280,6 +283,7 @@
       <color rgb="FFFFA6A6"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -287,18 +291,21 @@
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -306,6 +313,7 @@
       <color rgb="FF729FCF"/>
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -313,12 +321,14 @@
       <color rgb="FF729FCF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF729FCF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -326,12 +336,14 @@
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -339,18 +351,21 @@
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFBFBFBF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -358,6 +373,7 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -891,7 +907,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1393,8 +1409,8 @@
   </sheetPr>
   <dimension ref="A1:AY40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q22" activeCellId="0" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3035,8 +3051,8 @@
       <c r="R18" s="41"/>
       <c r="S18" s="41"/>
       <c r="T18" s="41"/>
-      <c r="U18" s="131" t="s">
-        <v>60</v>
+      <c r="U18" s="72" t="n">
+        <v>0.37</v>
       </c>
       <c r="V18" s="72" t="n">
         <v>1.08</v>
@@ -3050,7 +3066,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="134" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="135"/>
       <c r="C19" s="46"/>
@@ -3097,7 +3113,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="138" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="139"/>
       <c r="C20" s="140"/>

</xml_diff>

<commit_message>
change the name of (0) to be the files that olready run and without (1) to be runinig from the begining of teh cells
</commit_message>
<xml_diff>
--- a/cells_initial_information/Data2.xlsx
+++ b/cells_initial_information/Data2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t xml:space="preserve">cell_name</t>
   </si>
@@ -34,6 +34,15 @@
     <t xml:space="preserve">synapse ID</t>
   </si>
   <si>
+    <t xml:space="preserve">channel2take_presynaptic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel2take_postsynaptic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel2take_IV</t>
+  </si>
+  <si>
     <t xml:space="preserve">dis_from_soma</t>
   </si>
   <si>
@@ -130,7 +139,7 @@
     <t xml:space="preserve">last stable sweep</t>
   </si>
   <si>
-    <t xml:space="preserve">04_16_A</t>
+    <t xml:space="preserve">2016_04_16_A</t>
   </si>
   <si>
     <t xml:space="preserve">C8</t>
@@ -142,16 +151,16 @@
     <t xml:space="preserve">C6/7</t>
   </si>
   <si>
-    <t xml:space="preserve">05_12_A</t>
+    <t xml:space="preserve">2016_05_12_A</t>
   </si>
   <si>
     <t xml:space="preserve">basal</t>
   </si>
   <si>
-    <t xml:space="preserve">08_30_A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02_20_B</t>
+    <t xml:space="preserve">2016_08_30_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_02_20_B</t>
   </si>
   <si>
     <t xml:space="preserve">2017_03_04_A_6-7</t>
@@ -169,7 +178,7 @@
     <t xml:space="preserve">(873.38; 331.97; -289.32)</t>
   </si>
   <si>
-    <t xml:space="preserve">04_03_B</t>
+    <t xml:space="preserve">2017_04_03_B</t>
   </si>
   <si>
     <t xml:space="preserve">2017_05_08_A_4-5</t>
@@ -184,7 +193,7 @@
     <t xml:space="preserve">(-35.92; -391.47; -431.60)</t>
   </si>
   <si>
-    <t xml:space="preserve">07_06_C (3-&gt;4)</t>
+    <t xml:space="preserve">2017_07_06_C_3_4</t>
   </si>
   <si>
     <t xml:space="preserve">c112</t>
@@ -193,7 +202,7 @@
     <t xml:space="preserve">c69</t>
   </si>
   <si>
-    <t xml:space="preserve">07_06_C (4-&gt;3)</t>
+    <t xml:space="preserve">2017_07_06_C_4_3</t>
   </si>
   <si>
     <t xml:space="preserve">c301</t>
@@ -216,7 +225,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -276,6 +285,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FFFF972F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -549,52 +572,17 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="hair"/>
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
-      <bottom style="medium"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="medium"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -602,6 +590,48 @@
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -640,13 +670,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
       <right/>
       <top/>
@@ -661,10 +684,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
+      <left style="medium"/>
       <right/>
       <top/>
-      <bottom style="hair"/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -693,7 +716,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="168">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -918,7 +941,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -938,7 +965,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -946,39 +973,39 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -986,27 +1013,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1022,39 +1049,43 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1062,75 +1093,71 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="13" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="13" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1162,40 +1189,68 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="13" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1206,15 +1261,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1238,7 +1293,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1246,19 +1301,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1266,10 +1321,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1278,23 +1329,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1306,6 +1357,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1314,7 +1373,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1322,7 +1381,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1407,10 +1466,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AY40"/>
+  <dimension ref="A1:BB41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q22" activeCellId="0" sqref="Q22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1419,33 +1478,36 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="9"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="32.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="7.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="2" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="30.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="20.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="19" style="2" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="16.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="25" style="2" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="7.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="2" width="7.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="2" width="8.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="18.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="17.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="32.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="17.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="7.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="2" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="30.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="22" style="2" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="16.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="30" min="28" style="2" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="7.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="2" width="6.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="2" width="7.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="2" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="2" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="2" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="52" style="2" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="2" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="2" width="8.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="2" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="2" width="6.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="2" width="7.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="2" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="2" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="16.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="55" style="2" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1461,76 +1523,76 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="11" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="12" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="W1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="X1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="Z1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AA1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AB1" s="18" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="19" t="s">
@@ -1545,22 +1607,31 @@
       <c r="AF1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="20" t="s">
+      <c r="AG1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AH1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="16" t="s">
+      <c r="AI1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="16" t="s">
+      <c r="AJ1" s="20" t="s">
         <v>35</v>
+      </c>
+      <c r="AK1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>5</v>
@@ -1569,90 +1640,99 @@
         <v>2</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="25" t="n">
+        <v>40</v>
+      </c>
+      <c r="E2" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="25" t="n">
         <v>115.3</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26" t="n">
+      <c r="I2" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26" t="n">
         <v>0.154</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="25" t="n">
+      <c r="N2" s="27"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="25" t="n">
         <v>0.212</v>
       </c>
-      <c r="N2" s="25" t="n">
+      <c r="Q2" s="25" t="n">
         <v>0.164</v>
       </c>
-      <c r="O2" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" s="25" t="n">
+      <c r="R2" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" s="25" t="n">
         <v>0.106153386</v>
       </c>
-      <c r="Q2" s="25" t="n">
+      <c r="T2" s="25" t="n">
         <v>0.10058820047</v>
       </c>
-      <c r="R2" s="25" t="n">
+      <c r="U2" s="25" t="n">
         <v>0.00556518553</v>
       </c>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="0"/>
-      <c r="W2" s="29" t="n">
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="29" t="n">
         <v>2.25071899894022</v>
       </c>
-      <c r="X2" s="30" t="n">
+      <c r="AA2" s="30" t="n">
         <v>0.334431171556731</v>
       </c>
-      <c r="Y2" s="29" t="n">
+      <c r="AB2" s="29" t="n">
         <v>11</v>
       </c>
-      <c r="Z2" s="29" t="n">
+      <c r="AC2" s="29" t="n">
         <v>0.810626260829957</v>
       </c>
-      <c r="AA2" s="29" t="n">
+      <c r="AD2" s="29" t="n">
         <v>0.262405219390073</v>
       </c>
-      <c r="AB2" s="29" t="n">
+      <c r="AE2" s="29" t="n">
         <v>5</v>
       </c>
-      <c r="AC2" s="29" t="n">
+      <c r="AF2" s="29" t="n">
         <v>20</v>
       </c>
-      <c r="AD2" s="29" t="n">
+      <c r="AG2" s="29" t="n">
         <v>0.6</v>
       </c>
-      <c r="AE2" s="29" t="n">
+      <c r="AH2" s="29" t="n">
         <v>0.9</v>
       </c>
-      <c r="AF2" s="29" t="n">
+      <c r="AI2" s="29" t="n">
         <v>0.1</v>
       </c>
-      <c r="AG2" s="31" t="n">
+      <c r="AJ2" s="31" t="n">
         <v>1.1</v>
       </c>
-      <c r="AH2" s="32" t="n">
+      <c r="AK2" s="32" t="n">
         <v>100</v>
       </c>
-      <c r="AI2" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="33" t="n">
+      <c r="AL2" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="33" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="3" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>5</v>
@@ -1661,61 +1741,67 @@
         <v>2</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="35" t="n">
+        <v>42</v>
+      </c>
+      <c r="E3" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="35" t="n">
         <v>108.3</v>
       </c>
-      <c r="F3" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36" t="n">
+      <c r="I3" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36" t="n">
         <v>0.112</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="39" t="n">
+      <c r="N3" s="37"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="39" t="n">
         <v>1.458</v>
       </c>
-      <c r="N3" s="35" t="n">
+      <c r="Q3" s="35" t="n">
         <v>0.086</v>
       </c>
-      <c r="O3" s="40" t="n">
+      <c r="R3" s="40" t="n">
         <v>19</v>
       </c>
-      <c r="P3" s="35" t="n">
+      <c r="S3" s="35" t="n">
         <v>0.08501654566</v>
       </c>
-      <c r="Q3" s="35" t="n">
+      <c r="T3" s="35" t="n">
         <v>0.06873692349</v>
       </c>
-      <c r="R3" s="35" t="n">
+      <c r="U3" s="35" t="n">
         <v>0.01627962217</v>
       </c>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="0"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="29"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="0"/>
       <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
+      <c r="AA3" s="30"/>
       <c r="AB3" s="29"/>
       <c r="AC3" s="29"/>
       <c r="AD3" s="29"/>
       <c r="AE3" s="29"/>
       <c r="AF3" s="29"/>
-      <c r="AG3" s="31"/>
-      <c r="AH3" s="32"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
       <c r="AI3" s="29"/>
-      <c r="AJ3" s="33"/>
-      <c r="AK3" s="0"/>
-      <c r="AL3" s="0"/>
-      <c r="AM3" s="0"/>
+      <c r="AJ3" s="31"/>
+      <c r="AK3" s="32"/>
+      <c r="AL3" s="29"/>
+      <c r="AM3" s="33"/>
       <c r="AN3" s="0"/>
       <c r="AO3" s="0"/>
       <c r="AP3" s="0"/>
@@ -1728,10 +1814,13 @@
       <c r="AW3" s="0"/>
       <c r="AX3" s="0"/>
       <c r="AY3" s="0"/>
+      <c r="AZ3" s="0"/>
+      <c r="BA3" s="0"/>
+      <c r="BB3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="42" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B4" s="43" t="n">
         <v>7</v>
@@ -1742,88 +1831,97 @@
       <c r="D4" s="45" t="n">
         <v>120</v>
       </c>
-      <c r="E4" s="46" t="n">
+      <c r="E4" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="46" t="n">
         <v>60.6</v>
       </c>
-      <c r="F4" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47" t="n">
+      <c r="I4" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47" t="n">
         <v>0.07</v>
       </c>
-      <c r="K4" s="48"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="46" t="n">
+      <c r="N4" s="48"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="46" t="n">
         <v>0.551</v>
       </c>
-      <c r="N4" s="46" t="n">
+      <c r="Q4" s="46" t="n">
         <v>0.081</v>
       </c>
-      <c r="O4" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="P4" s="46" t="n">
+      <c r="R4" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="S4" s="46" t="n">
         <v>0.05851126589</v>
       </c>
-      <c r="Q4" s="46" t="n">
+      <c r="T4" s="46" t="n">
         <v>0.05077091477</v>
       </c>
-      <c r="R4" s="46" t="n">
+      <c r="U4" s="46" t="n">
         <v>0.00774035112</v>
       </c>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="0"/>
-      <c r="W4" s="51" t="n">
+      <c r="V4" s="46"/>
+      <c r="W4" s="46"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="51" t="n">
         <v>0.617651910055206</v>
       </c>
-      <c r="X4" s="52" t="n">
+      <c r="AA4" s="52" t="n">
         <v>0.327990127847546</v>
       </c>
-      <c r="Y4" s="51" t="n">
+      <c r="AB4" s="51" t="n">
         <v>3</v>
       </c>
-      <c r="Z4" s="51" t="n">
+      <c r="AC4" s="51" t="n">
         <v>0.519937896919427</v>
       </c>
-      <c r="AA4" s="53" t="n">
+      <c r="AD4" s="53" t="n">
         <v>0.362810904904287</v>
       </c>
-      <c r="AB4" s="51" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC4" s="51" t="n">
+      <c r="AE4" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="51" t="n">
         <v>15</v>
       </c>
-      <c r="AD4" s="51" t="n">
+      <c r="AG4" s="51" t="n">
         <v>0.1</v>
       </c>
-      <c r="AE4" s="51" t="n">
+      <c r="AH4" s="51" t="n">
         <v>0.7</v>
       </c>
-      <c r="AF4" s="51" t="n">
+      <c r="AI4" s="51" t="n">
         <v>0.1</v>
       </c>
-      <c r="AG4" s="54" t="n">
+      <c r="AJ4" s="54" t="n">
         <v>0.9</v>
       </c>
-      <c r="AH4" s="55" t="n">
+      <c r="AK4" s="55" t="n">
         <v>200</v>
       </c>
-      <c r="AI4" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="52" t="n">
+      <c r="AL4" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="52" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42" t="s">
-        <v>40</v>
+      <c r="A5" s="56" t="s">
+        <v>43</v>
       </c>
       <c r="B5" s="43" t="n">
         <v>7</v>
@@ -1834,152 +1932,170 @@
       <c r="D5" s="45" t="n">
         <v>202</v>
       </c>
-      <c r="E5" s="46" t="n">
+      <c r="E5" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="46" t="n">
         <v>64.9</v>
       </c>
-      <c r="F5" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47" t="n">
+      <c r="I5" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47" t="n">
         <v>0.065</v>
       </c>
-      <c r="K5" s="48"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="46" t="n">
+      <c r="N5" s="48"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="46" t="n">
         <v>0.94</v>
       </c>
-      <c r="N5" s="46" t="n">
+      <c r="Q5" s="46" t="n">
         <v>0.184</v>
       </c>
-      <c r="O5" s="50" t="n">
+      <c r="R5" s="50" t="n">
         <v>8</v>
       </c>
-      <c r="P5" s="46" t="n">
+      <c r="S5" s="46" t="n">
         <v>0.13098365934</v>
       </c>
-      <c r="Q5" s="46" t="n">
+      <c r="T5" s="46" t="n">
         <v>0.10212437501</v>
       </c>
-      <c r="R5" s="46" t="n">
+      <c r="U5" s="46" t="n">
         <v>0.02885928433</v>
       </c>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="0"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="51"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="0"/>
       <c r="Z5" s="51"/>
-      <c r="AA5" s="51"/>
+      <c r="AA5" s="52"/>
       <c r="AB5" s="51"/>
       <c r="AC5" s="51"/>
       <c r="AD5" s="51"/>
       <c r="AE5" s="51"/>
       <c r="AF5" s="51"/>
-      <c r="AG5" s="54"/>
-      <c r="AH5" s="55"/>
+      <c r="AG5" s="51"/>
+      <c r="AH5" s="51"/>
       <c r="AI5" s="51"/>
-      <c r="AJ5" s="52"/>
+      <c r="AJ5" s="54"/>
+      <c r="AK5" s="55"/>
+      <c r="AL5" s="51"/>
+      <c r="AM5" s="52"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="57" t="n">
+      <c r="A6" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="58" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="58" t="n">
+      <c r="C6" s="59" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="35" t="n">
+      <c r="E6" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="35" t="n">
         <v>68.4</v>
       </c>
-      <c r="F6" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36" t="n">
+      <c r="I6" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36" t="n">
         <v>0.031</v>
       </c>
-      <c r="K6" s="37"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="35" t="n">
+      <c r="N6" s="37"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="35" t="n">
         <v>0.644</v>
       </c>
-      <c r="N6" s="35" t="n">
+      <c r="Q6" s="35" t="n">
         <v>0.229</v>
       </c>
-      <c r="O6" s="40" t="n">
+      <c r="R6" s="40" t="n">
         <v>10</v>
       </c>
-      <c r="P6" s="35" t="n">
+      <c r="S6" s="35" t="n">
         <v>0.06421205609</v>
       </c>
-      <c r="Q6" s="35" t="n">
+      <c r="T6" s="35" t="n">
         <v>0.03222031342</v>
       </c>
-      <c r="R6" s="35" t="n">
+      <c r="U6" s="35" t="n">
         <v>0.03199174267</v>
       </c>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="0"/>
-      <c r="W6" s="35" t="n">
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="0"/>
+      <c r="Z6" s="35" t="n">
         <v>0.410064193382618</v>
       </c>
-      <c r="X6" s="38" t="n">
+      <c r="AA6" s="38" t="n">
         <v>0.190167451046957</v>
       </c>
-      <c r="Y6" s="59" t="n">
+      <c r="AB6" s="60" t="n">
         <v>4</v>
       </c>
-      <c r="Z6" s="59" t="n">
+      <c r="AC6" s="60" t="n">
         <v>0.569423206285454</v>
       </c>
-      <c r="AA6" s="59" t="n">
+      <c r="AD6" s="60" t="n">
         <v>0.204818840259996</v>
       </c>
-      <c r="AB6" s="59" t="n">
+      <c r="AE6" s="60" t="n">
         <v>3</v>
       </c>
-      <c r="AC6" s="59" t="n">
+      <c r="AF6" s="60" t="n">
         <v>16</v>
       </c>
-      <c r="AD6" s="59" t="n">
+      <c r="AG6" s="60" t="n">
         <v>0.4</v>
       </c>
-      <c r="AE6" s="59" t="n">
+      <c r="AH6" s="60" t="n">
         <v>0.8</v>
       </c>
-      <c r="AF6" s="59" t="n">
+      <c r="AI6" s="60" t="n">
         <v>0.1</v>
       </c>
-      <c r="AG6" s="31" t="n">
+      <c r="AJ6" s="31" t="n">
         <v>0.4</v>
       </c>
-      <c r="AH6" s="60" t="n">
+      <c r="AK6" s="61" t="n">
         <v>300</v>
       </c>
-      <c r="AI6" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="38" t="n">
+      <c r="AL6" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="38" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="s">
-        <v>43</v>
+      <c r="A7" s="62" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="43" t="n">
         <v>6</v>
@@ -1990,88 +2106,97 @@
       <c r="D7" s="45" t="n">
         <v>120</v>
       </c>
-      <c r="E7" s="46" t="n">
+      <c r="E7" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="46" t="n">
         <v>78.3</v>
       </c>
-      <c r="F7" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47" t="n">
+      <c r="I7" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47" t="n">
         <v>0.034</v>
       </c>
-      <c r="K7" s="48"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="46" t="n">
+      <c r="N7" s="48"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="46" t="n">
         <v>0.324</v>
       </c>
-      <c r="N7" s="46" t="n">
+      <c r="Q7" s="46" t="n">
         <v>0.087</v>
       </c>
-      <c r="O7" s="50" t="n">
+      <c r="R7" s="50" t="n">
         <v>5</v>
       </c>
-      <c r="P7" s="46" t="n">
+      <c r="S7" s="46" t="n">
         <v>0.02013426362</v>
       </c>
-      <c r="Q7" s="46" t="n">
+      <c r="T7" s="46" t="n">
         <v>0.0174641416</v>
       </c>
-      <c r="R7" s="46" t="n">
+      <c r="U7" s="46" t="n">
         <v>0.00267012202</v>
       </c>
-      <c r="S7" s="46"/>
-      <c r="T7" s="46"/>
-      <c r="U7" s="46"/>
-      <c r="V7" s="0"/>
-      <c r="W7" s="51" t="n">
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="51" t="n">
         <v>0.659842323569883</v>
       </c>
-      <c r="X7" s="52" t="n">
+      <c r="AA7" s="52" t="n">
         <v>0.271608046048613</v>
       </c>
-      <c r="Y7" s="51" t="n">
+      <c r="AB7" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="Z7" s="51" t="n">
+      <c r="AC7" s="51" t="n">
         <v>0.515806677611508</v>
       </c>
-      <c r="AA7" s="51" t="n">
+      <c r="AD7" s="51" t="n">
         <v>0.230901257526501</v>
       </c>
-      <c r="AB7" s="51" t="n">
+      <c r="AE7" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="AC7" s="51" t="n">
+      <c r="AF7" s="51" t="n">
         <v>19</v>
       </c>
-      <c r="AD7" s="51" t="n">
+      <c r="AG7" s="51" t="n">
         <v>0.1</v>
       </c>
-      <c r="AE7" s="51" t="n">
+      <c r="AH7" s="51" t="n">
         <v>0.8</v>
       </c>
-      <c r="AF7" s="51" t="n">
+      <c r="AI7" s="51" t="n">
         <v>0.1</v>
       </c>
-      <c r="AG7" s="54" t="n">
+      <c r="AJ7" s="54" t="n">
         <v>0.8</v>
       </c>
-      <c r="AH7" s="62" t="n">
+      <c r="AK7" s="63" t="n">
         <v>125</v>
       </c>
-      <c r="AI7" s="51" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ7" s="52" t="n">
+      <c r="AL7" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="52" t="n">
         <v>125</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="61" t="s">
-        <v>43</v>
+      <c r="A8" s="62" t="s">
+        <v>46</v>
       </c>
       <c r="B8" s="43" t="n">
         <v>6</v>
@@ -2082,163 +2207,178 @@
       <c r="D8" s="45" t="n">
         <v>191</v>
       </c>
-      <c r="E8" s="46" t="n">
+      <c r="E8" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="46" t="n">
         <v>88.7</v>
       </c>
-      <c r="F8" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47" t="n">
+      <c r="I8" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47" t="n">
         <v>0.027</v>
       </c>
-      <c r="K8" s="48"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="46" t="n">
+      <c r="N8" s="48"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="46" t="n">
         <v>0.642</v>
       </c>
-      <c r="N8" s="46" t="n">
+      <c r="Q8" s="46" t="n">
         <v>0.154</v>
       </c>
-      <c r="O8" s="50" t="n">
+      <c r="R8" s="50" t="n">
         <v>7</v>
       </c>
-      <c r="P8" s="46" t="n">
+      <c r="S8" s="46" t="n">
         <v>0.03974799833</v>
       </c>
-      <c r="Q8" s="46" t="n">
+      <c r="T8" s="46" t="n">
         <v>0.02970077495</v>
       </c>
-      <c r="R8" s="46" t="n">
+      <c r="U8" s="46" t="n">
         <v>0.01004722338</v>
       </c>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="0"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="52"/>
-      <c r="Y8" s="51"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="46"/>
+      <c r="Y8" s="0"/>
       <c r="Z8" s="51"/>
-      <c r="AA8" s="51"/>
+      <c r="AA8" s="52"/>
       <c r="AB8" s="51"/>
       <c r="AC8" s="51"/>
       <c r="AD8" s="51"/>
       <c r="AE8" s="51"/>
       <c r="AF8" s="51"/>
-      <c r="AG8" s="54"/>
-      <c r="AH8" s="62"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="51"/>
       <c r="AI8" s="51"/>
-      <c r="AJ8" s="52"/>
-    </row>
-    <row r="9" s="78" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="63" t="s">
+      <c r="AJ8" s="54"/>
+      <c r="AK8" s="63"/>
+      <c r="AL8" s="51"/>
+      <c r="AM8" s="52"/>
+    </row>
+    <row r="9" s="79" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="65" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="68" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="I9" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="64" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="65" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="67" t="n">
-        <v>32.6</v>
-      </c>
-      <c r="F9" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="68" t="n">
+      <c r="J9" s="69" t="n">
         <v>924.01</v>
       </c>
-      <c r="H9" s="68" t="n">
+      <c r="K9" s="69" t="n">
         <v>333.54</v>
       </c>
-      <c r="I9" s="68" t="n">
+      <c r="L9" s="69" t="n">
         <v>-257.4</v>
       </c>
-      <c r="J9" s="68" t="n">
+      <c r="M9" s="69" t="n">
         <v>0.114</v>
       </c>
-      <c r="K9" s="69" t="n">
+      <c r="N9" s="70" t="n">
         <v>199</v>
       </c>
-      <c r="L9" s="70" t="s">
-        <v>46</v>
-      </c>
-      <c r="M9" s="67" t="n">
+      <c r="O9" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="68" t="n">
         <v>0.763</v>
       </c>
-      <c r="N9" s="67" t="n">
+      <c r="Q9" s="68" t="n">
         <v>0.134</v>
       </c>
-      <c r="O9" s="71" t="n">
-        <v>1</v>
-      </c>
-      <c r="P9" s="67" t="n">
+      <c r="R9" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" s="68" t="n">
         <v>0.08501695029</v>
       </c>
-      <c r="Q9" s="67" t="n">
+      <c r="T9" s="68" t="n">
         <v>0.0745871871</v>
       </c>
-      <c r="R9" s="67" t="n">
+      <c r="U9" s="68" t="n">
         <v>0.01042976319</v>
       </c>
-      <c r="S9" s="67"/>
-      <c r="T9" s="67"/>
-      <c r="U9" s="67"/>
-      <c r="V9" s="72" t="n">
+      <c r="V9" s="68"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="68"/>
+      <c r="Y9" s="73" t="n">
         <v>1.08</v>
       </c>
-      <c r="W9" s="73" t="n">
+      <c r="Z9" s="74" t="n">
         <v>1.85989007744307</v>
       </c>
-      <c r="X9" s="73" t="n">
+      <c r="AA9" s="74" t="n">
         <v>0.324348142228853</v>
       </c>
-      <c r="Y9" s="0" t="n">
+      <c r="AB9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="Z9" s="73" t="n">
+      <c r="AC9" s="74" t="n">
         <v>0.805034067065075</v>
       </c>
-      <c r="AA9" s="73" t="n">
+      <c r="AD9" s="74" t="n">
         <v>0.290119432876338</v>
       </c>
-      <c r="AB9" s="74" t="n">
+      <c r="AE9" s="75" t="n">
         <v>5</v>
       </c>
-      <c r="AC9" s="74" t="n">
+      <c r="AF9" s="75" t="n">
         <v>20</v>
-      </c>
-      <c r="AD9" s="74" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="AE9" s="74" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="AF9" s="74" t="n">
-        <v>0.1</v>
       </c>
       <c r="AG9" s="75" t="n">
         <v>0.7</v>
       </c>
-      <c r="AH9" s="76" t="n">
+      <c r="AH9" s="75" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AI9" s="75" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AJ9" s="76" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AK9" s="77" t="n">
         <v>200</v>
       </c>
-      <c r="AI9" s="74" t="n">
+      <c r="AL9" s="75" t="n">
         <v>26</v>
       </c>
-      <c r="AJ9" s="77" t="n">
+      <c r="AM9" s="78" t="n">
         <v>225</v>
       </c>
-      <c r="AK9" s="0"/>
-      <c r="AL9" s="0"/>
-      <c r="AM9" s="0"/>
       <c r="AN9" s="0"/>
       <c r="AO9" s="0"/>
       <c r="AP9" s="0"/>
@@ -2251,95 +2391,104 @@
       <c r="AW9" s="0"/>
       <c r="AX9" s="0"/>
       <c r="AY9" s="0"/>
-    </row>
-    <row r="10" s="78" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="63" t="s">
+      <c r="AZ9" s="0"/>
+      <c r="BA9" s="0"/>
+      <c r="BB9" s="0"/>
+    </row>
+    <row r="10" s="79" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="65" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="68" t="n">
+        <v>50.6</v>
+      </c>
+      <c r="I10" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="64" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="65" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="67" t="n">
-        <v>50.6</v>
-      </c>
-      <c r="F10" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="68" t="n">
+      <c r="J10" s="69" t="n">
         <v>873.38</v>
       </c>
-      <c r="H10" s="68" t="n">
+      <c r="K10" s="69" t="n">
         <v>331.97</v>
       </c>
-      <c r="I10" s="68" t="n">
+      <c r="L10" s="69" t="n">
         <v>-289.32</v>
       </c>
-      <c r="J10" s="68" t="n">
+      <c r="M10" s="69" t="n">
         <v>0.039</v>
       </c>
-      <c r="K10" s="69" t="n">
+      <c r="N10" s="70" t="n">
         <v>3806</v>
       </c>
-      <c r="L10" s="70" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" s="67" t="n">
+      <c r="O10" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" s="68" t="n">
         <v>0.905</v>
       </c>
-      <c r="N10" s="67" t="n">
+      <c r="Q10" s="68" t="n">
         <v>0.085</v>
       </c>
-      <c r="O10" s="71" t="n">
-        <v>1</v>
-      </c>
-      <c r="P10" s="67" t="n">
+      <c r="R10" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" s="68" t="n">
         <v>0.0783942101</v>
       </c>
-      <c r="Q10" s="67" t="n">
+      <c r="T10" s="68" t="n">
         <v>0.06459193692</v>
       </c>
-      <c r="R10" s="67" t="n">
+      <c r="U10" s="68" t="n">
         <v>0.01380227318</v>
       </c>
-      <c r="S10" s="67"/>
-      <c r="T10" s="67"/>
-      <c r="U10" s="67"/>
-      <c r="V10" s="72" t="n">
+      <c r="V10" s="68"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="68"/>
+      <c r="Y10" s="73" t="n">
         <v>1.08</v>
       </c>
-      <c r="W10" s="74" t="n">
+      <c r="Z10" s="75" t="n">
         <v>1.85989007744307</v>
       </c>
-      <c r="X10" s="77" t="n">
+      <c r="AA10" s="78" t="n">
         <v>0.324348142228853</v>
       </c>
-      <c r="Y10" s="74" t="n">
+      <c r="AB10" s="75" t="n">
         <v>8</v>
       </c>
-      <c r="Z10" s="74" t="n">
+      <c r="AC10" s="75" t="n">
         <v>0.805034067065075</v>
       </c>
-      <c r="AA10" s="74" t="n">
+      <c r="AD10" s="75" t="n">
         <v>0.290119432876338</v>
       </c>
-      <c r="AB10" s="74"/>
-      <c r="AC10" s="74"/>
-      <c r="AD10" s="74"/>
-      <c r="AE10" s="74"/>
-      <c r="AF10" s="74"/>
+      <c r="AE10" s="75"/>
+      <c r="AF10" s="75"/>
       <c r="AG10" s="75"/>
-      <c r="AH10" s="76"/>
-      <c r="AI10" s="74"/>
-      <c r="AJ10" s="77"/>
-      <c r="AK10" s="0"/>
-      <c r="AL10" s="0"/>
-      <c r="AM10" s="0"/>
+      <c r="AH10" s="75"/>
+      <c r="AI10" s="75"/>
+      <c r="AJ10" s="76"/>
+      <c r="AK10" s="77"/>
+      <c r="AL10" s="75"/>
+      <c r="AM10" s="78"/>
       <c r="AN10" s="0"/>
       <c r="AO10" s="0"/>
       <c r="AP10" s="0"/>
@@ -2352,201 +2501,219 @@
       <c r="AW10" s="0"/>
       <c r="AX10" s="0"/>
       <c r="AY10" s="0"/>
+      <c r="AZ10" s="0"/>
+      <c r="BA10" s="0"/>
+      <c r="BB10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="79" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="80" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="81" t="n">
+      <c r="A11" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="81" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="82" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="45" t="n">
         <v>70</v>
       </c>
-      <c r="E11" s="46" t="n">
+      <c r="E11" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="46" t="n">
         <v>113.9</v>
       </c>
-      <c r="F11" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47" t="n">
+      <c r="I11" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47" t="n">
         <v>0.109</v>
       </c>
-      <c r="K11" s="48"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="46" t="n">
+      <c r="N11" s="48"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="46" t="n">
         <v>0.823</v>
       </c>
-      <c r="N11" s="46" t="n">
+      <c r="Q11" s="46" t="n">
         <v>0.114</v>
       </c>
-      <c r="O11" s="46" t="n">
-        <v>1</v>
-      </c>
-      <c r="P11" s="46" t="n">
+      <c r="R11" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="S11" s="46" t="n">
         <v>0.12067868041</v>
       </c>
-      <c r="Q11" s="46" t="n">
+      <c r="T11" s="46" t="n">
         <v>0.10429282878</v>
       </c>
-      <c r="R11" s="46" t="n">
+      <c r="U11" s="46" t="n">
         <v>0.01638585163</v>
       </c>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="0"/>
-      <c r="W11" s="46" t="n">
+      <c r="V11" s="46"/>
+      <c r="W11" s="46"/>
+      <c r="X11" s="46"/>
+      <c r="Y11" s="0"/>
+      <c r="Z11" s="46" t="n">
         <v>1.00928476950415</v>
       </c>
-      <c r="X11" s="49" t="n">
+      <c r="AA11" s="49" t="n">
         <v>0.199208462943467</v>
       </c>
-      <c r="Y11" s="51" t="n">
+      <c r="AB11" s="51" t="n">
         <v>9</v>
       </c>
-      <c r="Z11" s="51" t="n">
+      <c r="AC11" s="51" t="n">
         <v>0.729963006834759</v>
       </c>
-      <c r="AA11" s="51" t="n">
+      <c r="AD11" s="51" t="n">
         <v>0.145605770201242</v>
       </c>
-      <c r="AB11" s="51" t="n">
+      <c r="AE11" s="51" t="n">
         <v>5</v>
       </c>
-      <c r="AC11" s="51" t="n">
+      <c r="AF11" s="51" t="n">
         <v>20</v>
       </c>
-      <c r="AD11" s="51" t="n">
+      <c r="AG11" s="51" t="n">
         <v>0.5</v>
       </c>
-      <c r="AE11" s="51" t="n">
+      <c r="AH11" s="51" t="n">
         <v>0.9</v>
       </c>
-      <c r="AF11" s="51" t="n">
+      <c r="AI11" s="51" t="n">
         <v>0.1</v>
       </c>
-      <c r="AG11" s="54" t="n">
+      <c r="AJ11" s="54" t="n">
         <v>0.5</v>
       </c>
-      <c r="AH11" s="55" t="n">
+      <c r="AK11" s="55" t="n">
         <v>175</v>
       </c>
-      <c r="AI11" s="46" t="n">
+      <c r="AL11" s="46" t="n">
         <v>151</v>
       </c>
-      <c r="AJ11" s="49" t="n">
+      <c r="AM11" s="49" t="n">
         <v>325</v>
       </c>
     </row>
-    <row r="12" s="96" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="83" t="n">
+    <row r="12" s="97" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="83" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="84" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="84" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="85" t="n">
+      <c r="C12" s="85" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="86" t="n">
         <v>91</v>
       </c>
       <c r="E12" s="86" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="86" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="86" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="87" t="n">
         <v>83.8</v>
       </c>
-      <c r="F12" s="86" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="87" t="n">
+      <c r="I12" s="87" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="88" t="n">
         <v>-5.56</v>
       </c>
-      <c r="H12" s="87" t="n">
+      <c r="K12" s="88" t="n">
         <v>-325.88</v>
       </c>
-      <c r="I12" s="88" t="n">
+      <c r="L12" s="89" t="n">
         <v>-451.42</v>
       </c>
-      <c r="J12" s="89" t="n">
+      <c r="M12" s="90" t="n">
         <v>0.14</v>
       </c>
-      <c r="K12" s="90" t="n">
+      <c r="N12" s="91" t="n">
         <v>82</v>
       </c>
-      <c r="L12" s="91"/>
-      <c r="M12" s="86" t="n">
+      <c r="O12" s="92"/>
+      <c r="P12" s="87" t="n">
         <v>0.782</v>
       </c>
-      <c r="N12" s="86" t="n">
+      <c r="Q12" s="87" t="n">
         <v>0.164</v>
       </c>
-      <c r="O12" s="86" t="n">
+      <c r="R12" s="87" t="n">
         <v>11</v>
       </c>
-      <c r="P12" s="86" t="n">
+      <c r="S12" s="87" t="n">
         <v>0.16884774101</v>
       </c>
-      <c r="Q12" s="86" t="n">
+      <c r="T12" s="87" t="n">
         <v>0.13906972096</v>
       </c>
-      <c r="R12" s="86" t="n">
+      <c r="U12" s="87" t="n">
         <v>0.02977802005</v>
       </c>
-      <c r="S12" s="86"/>
-      <c r="T12" s="86"/>
-      <c r="U12" s="86"/>
-      <c r="V12" s="0"/>
-      <c r="W12" s="86" t="n">
+      <c r="V12" s="87"/>
+      <c r="W12" s="87"/>
+      <c r="X12" s="87"/>
+      <c r="Y12" s="0"/>
+      <c r="Z12" s="87" t="n">
         <v>1.26083037757995</v>
       </c>
-      <c r="X12" s="92" t="n">
+      <c r="AA12" s="93" t="n">
         <v>0.417980287594169</v>
       </c>
-      <c r="Y12" s="93" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="93" t="n">
+      <c r="AB12" s="94" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="94" t="n">
         <v>0.794059892657374</v>
       </c>
-      <c r="AA12" s="93" t="n">
+      <c r="AD12" s="94" t="n">
         <v>0.67284340860646</v>
       </c>
-      <c r="AB12" s="93" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC12" s="93" t="n">
+      <c r="AE12" s="94" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF12" s="94" t="n">
         <v>14</v>
       </c>
-      <c r="AD12" s="93" t="n">
+      <c r="AG12" s="94" t="n">
         <v>0.7</v>
       </c>
-      <c r="AE12" s="93" t="n">
+      <c r="AH12" s="94" t="n">
         <v>0.9</v>
       </c>
-      <c r="AF12" s="93" t="n">
+      <c r="AI12" s="94" t="n">
         <v>0.2</v>
       </c>
-      <c r="AG12" s="94" t="n">
+      <c r="AJ12" s="95" t="n">
         <v>1.2</v>
       </c>
-      <c r="AH12" s="95" t="n">
+      <c r="AK12" s="96" t="n">
         <v>275</v>
       </c>
-      <c r="AI12" s="86" t="n">
+      <c r="AL12" s="87" t="n">
         <v>176</v>
       </c>
-      <c r="AJ12" s="92" t="n">
+      <c r="AM12" s="93" t="n">
         <v>450</v>
       </c>
-      <c r="AK12" s="0"/>
-      <c r="AL12" s="0"/>
-      <c r="AM12" s="0"/>
       <c r="AN12" s="0"/>
       <c r="AO12" s="0"/>
       <c r="AP12" s="0"/>
@@ -2559,113 +2726,122 @@
       <c r="AW12" s="0"/>
       <c r="AX12" s="0"/>
       <c r="AY12" s="0"/>
-    </row>
-    <row r="13" s="109" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="97" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="98" t="n">
+      <c r="AZ12" s="0"/>
+      <c r="BA12" s="0"/>
+      <c r="BB12" s="0"/>
+    </row>
+    <row r="13" s="110" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="98" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="99" t="n">
         <v>4</v>
       </c>
-      <c r="C13" s="99" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" s="100" t="n">
+      <c r="C13" s="100" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="101" t="n">
         <v>42</v>
       </c>
       <c r="E13" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="102" t="n">
         <v>77.5</v>
       </c>
-      <c r="F13" s="101" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="102" t="n">
+      <c r="I13" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="103" t="n">
         <v>-31.93</v>
       </c>
-      <c r="H13" s="102" t="n">
+      <c r="K13" s="103" t="n">
         <v>-355.4</v>
       </c>
-      <c r="I13" s="102" t="n">
+      <c r="L13" s="103" t="n">
         <v>-423.02</v>
       </c>
-      <c r="J13" s="102" t="n">
+      <c r="M13" s="103" t="n">
         <v>0.066</v>
       </c>
-      <c r="K13" s="103" t="n">
+      <c r="N13" s="104" t="n">
         <v>4358</v>
       </c>
-      <c r="L13" s="104" t="s">
-        <v>52</v>
-      </c>
-      <c r="M13" s="101" t="n">
+      <c r="O13" s="105" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" s="102" t="n">
         <v>1.266</v>
       </c>
-      <c r="N13" s="101" t="n">
+      <c r="Q13" s="102" t="n">
         <v>0.125</v>
       </c>
-      <c r="O13" s="101" t="n">
+      <c r="R13" s="102" t="n">
         <v>15</v>
       </c>
-      <c r="P13" s="101" t="n">
+      <c r="S13" s="102" t="n">
         <v>0.06818310193</v>
       </c>
-      <c r="Q13" s="101" t="n">
+      <c r="T13" s="102" t="n">
         <v>0.03371715503</v>
       </c>
-      <c r="R13" s="101" t="n">
+      <c r="U13" s="102" t="n">
         <v>0.0344659469</v>
       </c>
-      <c r="S13" s="101"/>
-      <c r="T13" s="101"/>
-      <c r="U13" s="101"/>
-      <c r="V13" s="72" t="n">
+      <c r="V13" s="102"/>
+      <c r="W13" s="102"/>
+      <c r="X13" s="102"/>
+      <c r="Y13" s="73" t="n">
         <v>1.08</v>
       </c>
-      <c r="W13" s="105" t="n">
+      <c r="Z13" s="106" t="n">
         <v>1.70290313569153</v>
       </c>
-      <c r="X13" s="105" t="n">
+      <c r="AA13" s="106" t="n">
         <v>0.33438126301574</v>
       </c>
-      <c r="Y13" s="105" t="n">
+      <c r="AB13" s="106" t="n">
         <v>16</v>
       </c>
-      <c r="Z13" s="105" t="n">
+      <c r="AC13" s="106" t="n">
         <v>0.620744947626598</v>
       </c>
-      <c r="AA13" s="105" t="n">
+      <c r="AD13" s="106" t="n">
         <v>0.173126100637382</v>
       </c>
-      <c r="AB13" s="105" t="n">
+      <c r="AE13" s="106" t="n">
         <v>8</v>
       </c>
-      <c r="AC13" s="105" t="n">
+      <c r="AF13" s="106" t="n">
         <v>20</v>
-      </c>
-      <c r="AD13" s="105" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="AE13" s="105" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="AF13" s="105" t="n">
-        <v>0.1</v>
       </c>
       <c r="AG13" s="106" t="n">
         <v>0.4</v>
       </c>
-      <c r="AH13" s="107" t="n">
+      <c r="AH13" s="106" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AI13" s="106" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AJ13" s="107" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AK13" s="108" t="n">
         <v>325</v>
       </c>
-      <c r="AI13" s="105" t="n">
+      <c r="AL13" s="106" t="n">
         <v>126</v>
       </c>
-      <c r="AJ13" s="108" t="n">
+      <c r="AM13" s="109" t="n">
         <v>450</v>
       </c>
-      <c r="AK13" s="0"/>
-      <c r="AL13" s="0"/>
-      <c r="AM13" s="0"/>
       <c r="AN13" s="0"/>
       <c r="AO13" s="0"/>
       <c r="AP13" s="0"/>
@@ -2678,95 +2854,104 @@
       <c r="AW13" s="0"/>
       <c r="AX13" s="0"/>
       <c r="AY13" s="0"/>
-    </row>
-    <row r="14" s="109" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="97" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="98" t="n">
+      <c r="AZ13" s="0"/>
+      <c r="BA13" s="0"/>
+      <c r="BB13" s="0"/>
+    </row>
+    <row r="14" s="110" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="98" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="99" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="99" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" s="100" t="n">
+      <c r="C14" s="100" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="101" t="n">
         <v>68</v>
       </c>
       <c r="E14" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="102" t="n">
         <v>74.3</v>
       </c>
-      <c r="F14" s="101" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="102" t="n">
+      <c r="I14" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="103" t="n">
         <v>-35.92</v>
       </c>
-      <c r="H14" s="102" t="n">
+      <c r="K14" s="103" t="n">
         <v>-391.47</v>
       </c>
-      <c r="I14" s="102" t="n">
+      <c r="L14" s="103" t="n">
         <v>-431.6</v>
       </c>
-      <c r="J14" s="102" t="n">
+      <c r="M14" s="103" t="n">
         <v>0.014</v>
       </c>
-      <c r="K14" s="103" t="n">
+      <c r="N14" s="104" t="n">
         <v>3923</v>
       </c>
-      <c r="L14" s="104" t="s">
-        <v>53</v>
-      </c>
-      <c r="M14" s="101" t="n">
+      <c r="O14" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="102" t="n">
         <v>1.121</v>
       </c>
-      <c r="N14" s="101" t="n">
+      <c r="Q14" s="102" t="n">
         <v>0.102</v>
       </c>
-      <c r="O14" s="101" t="n">
+      <c r="R14" s="102" t="n">
         <v>13</v>
       </c>
-      <c r="P14" s="101" t="n">
+      <c r="S14" s="102" t="n">
         <v>0.02865474235</v>
       </c>
-      <c r="Q14" s="101" t="n">
+      <c r="T14" s="102" t="n">
         <v>0.01125841287</v>
       </c>
-      <c r="R14" s="101" t="n">
+      <c r="U14" s="102" t="n">
         <v>0.01739632948</v>
       </c>
-      <c r="S14" s="101"/>
-      <c r="T14" s="101"/>
-      <c r="U14" s="101"/>
-      <c r="V14" s="72" t="n">
+      <c r="V14" s="102"/>
+      <c r="W14" s="102"/>
+      <c r="X14" s="102"/>
+      <c r="Y14" s="73" t="n">
         <v>1.08</v>
       </c>
-      <c r="W14" s="105" t="n">
+      <c r="Z14" s="106" t="n">
         <v>1.70290313569153</v>
       </c>
-      <c r="X14" s="105" t="n">
+      <c r="AA14" s="106" t="n">
         <v>0.33438126301574</v>
       </c>
-      <c r="Y14" s="105" t="n">
+      <c r="AB14" s="106" t="n">
         <v>16</v>
       </c>
-      <c r="Z14" s="105" t="n">
+      <c r="AC14" s="106" t="n">
         <v>0.620744947626598</v>
       </c>
-      <c r="AA14" s="105" t="n">
+      <c r="AD14" s="106" t="n">
         <v>0.173126100637382</v>
       </c>
-      <c r="AB14" s="105"/>
-      <c r="AC14" s="105"/>
-      <c r="AD14" s="105"/>
-      <c r="AE14" s="105"/>
-      <c r="AF14" s="105"/>
+      <c r="AE14" s="106"/>
+      <c r="AF14" s="106"/>
       <c r="AG14" s="106"/>
-      <c r="AH14" s="107"/>
-      <c r="AI14" s="105"/>
-      <c r="AJ14" s="108"/>
-      <c r="AK14" s="0"/>
-      <c r="AL14" s="0"/>
-      <c r="AM14" s="0"/>
+      <c r="AH14" s="106"/>
+      <c r="AI14" s="106"/>
+      <c r="AJ14" s="107"/>
+      <c r="AK14" s="108"/>
+      <c r="AL14" s="106"/>
+      <c r="AM14" s="109"/>
       <c r="AN14" s="0"/>
       <c r="AO14" s="0"/>
       <c r="AP14" s="0"/>
@@ -2779,10 +2964,13 @@
       <c r="AW14" s="0"/>
       <c r="AX14" s="0"/>
       <c r="AY14" s="0"/>
+      <c r="AZ14" s="0"/>
+      <c r="BA14" s="0"/>
+      <c r="BB14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="110" t="s">
-        <v>54</v>
+      <c r="A15" s="111" t="s">
+        <v>57</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>5</v>
@@ -2790,32 +2978,32 @@
       <c r="C15" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="D15" s="111" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="35" t="n">
+      <c r="D15" s="112" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="112" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="112" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="112" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="35" t="n">
         <v>90.87</v>
       </c>
-      <c r="F15" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36" t="n">
+      <c r="I15" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36" t="n">
         <v>0.012</v>
       </c>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="N15" s="37"/>
+      <c r="O15" s="38"/>
       <c r="P15" s="35" t="n">
         <v>0</v>
       </c>
@@ -2825,56 +3013,65 @@
       <c r="R15" s="35" t="n">
         <v>0</v>
       </c>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="0"/>
-      <c r="W15" s="59" t="n">
+      <c r="S15" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
+      <c r="X15" s="35"/>
+      <c r="Y15" s="0"/>
+      <c r="Z15" s="60" t="n">
         <v>0.148073219653408</v>
       </c>
-      <c r="X15" s="112" t="n">
+      <c r="AA15" s="113" t="n">
         <v>0.144962080584371</v>
       </c>
-      <c r="Y15" s="59" t="n">
+      <c r="AB15" s="60" t="n">
         <v>6</v>
       </c>
-      <c r="Z15" s="59" t="n">
+      <c r="AC15" s="60" t="n">
         <v>0.14743558175711</v>
       </c>
-      <c r="AA15" s="59" t="n">
+      <c r="AD15" s="60" t="n">
         <v>0.166458165561462</v>
       </c>
-      <c r="AB15" s="59" t="n">
+      <c r="AE15" s="60" t="n">
         <v>4</v>
       </c>
-      <c r="AC15" s="59" t="n">
+      <c r="AF15" s="60" t="n">
         <v>19</v>
       </c>
-      <c r="AD15" s="59" t="n">
+      <c r="AG15" s="60" t="n">
         <v>0.1</v>
       </c>
-      <c r="AE15" s="59" t="n">
+      <c r="AH15" s="60" t="n">
         <v>0.5</v>
       </c>
-      <c r="AF15" s="59" t="n">
+      <c r="AI15" s="60" t="n">
         <v>0.1</v>
       </c>
-      <c r="AG15" s="31" t="n">
+      <c r="AJ15" s="31" t="n">
         <v>0.5</v>
       </c>
-      <c r="AH15" s="113" t="n">
+      <c r="AK15" s="114" t="n">
         <v>225</v>
       </c>
-      <c r="AI15" s="59" t="n">
+      <c r="AL15" s="60" t="n">
         <v>51</v>
       </c>
-      <c r="AJ15" s="112" t="n">
+      <c r="AM15" s="113" t="n">
         <v>275</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="114" t="s">
-        <v>54</v>
+      <c r="A16" s="115" t="s">
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>5</v>
@@ -2882,405 +3079,459 @@
       <c r="C16" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="D16" s="111" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="35" t="n">
+      <c r="D16" s="112" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="112" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="112" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="112" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" s="35" t="n">
         <v>235.05</v>
       </c>
-      <c r="F16" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36" t="n">
+      <c r="I16" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36" t="n">
         <v>0.064</v>
       </c>
-      <c r="K16" s="37"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="35" t="n">
+      <c r="N16" s="37"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="35" t="n">
         <v>0.806</v>
       </c>
-      <c r="N16" s="35" t="n">
+      <c r="Q16" s="35" t="n">
         <v>0.09</v>
       </c>
-      <c r="O16" s="35" t="n">
+      <c r="R16" s="35" t="n">
         <v>5</v>
       </c>
-      <c r="P16" s="35" t="n">
+      <c r="S16" s="35" t="n">
         <v>0.0508487542</v>
       </c>
-      <c r="Q16" s="35" t="n">
+      <c r="T16" s="35" t="n">
         <v>0.03783304638</v>
       </c>
-      <c r="R16" s="35" t="n">
+      <c r="U16" s="35" t="n">
         <v>0.01301570782</v>
       </c>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="0"/>
-      <c r="W16" s="59"/>
-      <c r="X16" s="112"/>
-      <c r="Y16" s="59"/>
-      <c r="Z16" s="59"/>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="59"/>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
-      <c r="AF16" s="59"/>
-      <c r="AG16" s="31"/>
-      <c r="AH16" s="113"/>
-      <c r="AI16" s="59"/>
-      <c r="AJ16" s="112"/>
+      <c r="V16" s="35"/>
+      <c r="W16" s="35"/>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="0"/>
+      <c r="Z16" s="60"/>
+      <c r="AA16" s="113"/>
+      <c r="AB16" s="60"/>
+      <c r="AC16" s="60"/>
+      <c r="AD16" s="60"/>
+      <c r="AE16" s="60"/>
+      <c r="AF16" s="60"/>
+      <c r="AG16" s="60"/>
+      <c r="AH16" s="60"/>
+      <c r="AI16" s="60"/>
+      <c r="AJ16" s="31"/>
+      <c r="AK16" s="114"/>
+      <c r="AL16" s="60"/>
+      <c r="AM16" s="113"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="115" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="116" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="117" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="118" t="s">
-        <v>58</v>
+      <c r="A17" s="116" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="117" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="119" t="s">
+        <v>61</v>
       </c>
       <c r="E17" s="119" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="120" t="n">
         <v>73.44</v>
       </c>
-      <c r="F17" s="119" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="120" t="n">
+      <c r="I17" s="120" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="121"/>
+      <c r="K17" s="121"/>
+      <c r="L17" s="121"/>
+      <c r="M17" s="121" t="n">
         <v>0.081</v>
       </c>
-      <c r="K17" s="121"/>
-      <c r="L17" s="122"/>
-      <c r="M17" s="119" t="n">
+      <c r="N17" s="122"/>
+      <c r="O17" s="123"/>
+      <c r="P17" s="120" t="n">
         <v>1.063</v>
       </c>
-      <c r="N17" s="119" t="n">
+      <c r="Q17" s="120" t="n">
         <v>0.117</v>
       </c>
-      <c r="O17" s="119" t="n">
+      <c r="R17" s="120" t="n">
         <v>7</v>
       </c>
-      <c r="P17" s="119" t="n">
+      <c r="S17" s="120" t="n">
         <v>0.09210808196</v>
       </c>
-      <c r="Q17" s="119" t="n">
+      <c r="T17" s="120" t="n">
         <v>0.0702311231</v>
       </c>
-      <c r="R17" s="119" t="n">
+      <c r="U17" s="120" t="n">
         <v>0.02187695886</v>
       </c>
-      <c r="S17" s="119"/>
-      <c r="T17" s="119"/>
-      <c r="U17" s="119"/>
-      <c r="V17" s="0"/>
-      <c r="W17" s="119" t="n">
+      <c r="V17" s="120"/>
+      <c r="W17" s="120"/>
+      <c r="X17" s="120"/>
+      <c r="Y17" s="124"/>
+      <c r="Z17" s="120" t="n">
         <v>0.585780971744615</v>
       </c>
-      <c r="X17" s="122" t="n">
+      <c r="AA17" s="123" t="n">
         <v>0.287981450721111</v>
       </c>
-      <c r="Y17" s="123" t="n">
+      <c r="AB17" s="125" t="n">
         <v>4</v>
       </c>
-      <c r="Z17" s="123" t="n">
+      <c r="AC17" s="125" t="n">
         <v>0.489876551485588</v>
       </c>
-      <c r="AA17" s="123" t="n">
+      <c r="AD17" s="125" t="n">
         <v>0.277535462267387</v>
       </c>
-      <c r="AB17" s="123" t="n">
+      <c r="AE17" s="125" t="n">
         <v>3</v>
       </c>
-      <c r="AC17" s="123" t="n">
+      <c r="AF17" s="125" t="n">
         <v>15</v>
       </c>
-      <c r="AD17" s="123" t="n">
+      <c r="AG17" s="125" t="n">
         <v>0.3</v>
       </c>
-      <c r="AE17" s="123" t="n">
+      <c r="AH17" s="125" t="n">
         <v>0.7</v>
       </c>
-      <c r="AF17" s="123" t="n">
+      <c r="AI17" s="125" t="n">
         <v>0.1</v>
       </c>
-      <c r="AG17" s="54" t="n">
+      <c r="AJ17" s="126" t="n">
         <v>0.5</v>
       </c>
-      <c r="AH17" s="124" t="n">
+      <c r="AK17" s="127" t="n">
         <v>325</v>
       </c>
-      <c r="AI17" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ17" s="125" t="n">
+      <c r="AL17" s="120" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM17" s="123" t="n">
         <v>325</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="126" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="127"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="G18" s="127"/>
-      <c r="H18" s="127"/>
-      <c r="I18" s="127"/>
-      <c r="K18" s="128"/>
-      <c r="M18" s="129" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="N18" s="130" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="O18" s="131"/>
-      <c r="P18" s="131"/>
-      <c r="Q18" s="0"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
-      <c r="U18" s="72" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="V18" s="72" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="W18" s="41"/>
-      <c r="AA18" s="0"/>
+      <c r="A18" s="128"/>
+      <c r="B18" s="129"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="131"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="132"/>
+      <c r="G18" s="132"/>
+      <c r="H18" s="132"/>
+      <c r="I18" s="132"/>
+      <c r="J18" s="132"/>
+      <c r="K18" s="132"/>
+      <c r="L18" s="132"/>
+      <c r="M18" s="132"/>
+      <c r="N18" s="132"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="132"/>
+      <c r="Q18" s="132"/>
+      <c r="R18" s="132"/>
+      <c r="S18" s="132"/>
+      <c r="T18" s="132"/>
+      <c r="U18" s="132"/>
+      <c r="V18" s="132"/>
+      <c r="W18" s="132"/>
+      <c r="X18" s="132"/>
+      <c r="Y18" s="132"/>
+      <c r="Z18" s="132"/>
+      <c r="AA18" s="132"/>
+      <c r="AB18" s="132"/>
+      <c r="AC18" s="132"/>
+      <c r="AD18" s="132"/>
+      <c r="AE18" s="132"/>
+      <c r="AF18" s="132"/>
       <c r="AG18" s="132"/>
-      <c r="AH18" s="41"/>
-      <c r="AI18" s="41"/>
-      <c r="AJ18" s="133"/>
+      <c r="AH18" s="132"/>
+      <c r="AI18" s="132"/>
+      <c r="AJ18" s="132"/>
+      <c r="AK18" s="132"/>
+      <c r="AL18" s="132"/>
+      <c r="AM18" s="133"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="134" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B19" s="135"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="135"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="135"/>
-      <c r="H19" s="135"/>
-      <c r="I19" s="135"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="136"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="135" t="n">
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="J19" s="135"/>
+      <c r="K19" s="135"/>
+      <c r="L19" s="135"/>
+      <c r="N19" s="136"/>
+      <c r="P19" s="137" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="Q19" s="138" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R19" s="139"/>
+      <c r="S19" s="139"/>
+      <c r="T19" s="0"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="73" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="Y19" s="73" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="Z19" s="41"/>
+      <c r="AD19" s="0"/>
+      <c r="AJ19" s="140"/>
+      <c r="AK19" s="41"/>
+      <c r="AL19" s="41"/>
+      <c r="AM19" s="141"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="142" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="143"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="143"/>
+      <c r="E20" s="143"/>
+      <c r="F20" s="143"/>
+      <c r="G20" s="143"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="143"/>
+      <c r="K20" s="143"/>
+      <c r="L20" s="143"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="144"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="143" t="n">
         <v>0.001</v>
       </c>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="46"/>
-      <c r="S19" s="46" t="n">
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="46"/>
+      <c r="V20" s="46" t="n">
         <v>0.944</v>
       </c>
-      <c r="T19" s="46" t="n">
+      <c r="W20" s="46" t="n">
         <f aca="false">0.944/2</f>
         <v>0.472</v>
       </c>
-      <c r="U19" s="46"/>
-      <c r="V19" s="46"/>
-      <c r="W19" s="46"/>
-      <c r="X19" s="46"/>
-      <c r="Y19" s="46"/>
-      <c r="Z19" s="46"/>
-      <c r="AA19" s="46"/>
-      <c r="AB19" s="46"/>
-      <c r="AC19" s="46"/>
-      <c r="AD19" s="46"/>
-      <c r="AE19" s="46"/>
-      <c r="AF19" s="46"/>
-      <c r="AG19" s="137"/>
-      <c r="AH19" s="46"/>
-      <c r="AI19" s="46"/>
-      <c r="AJ19" s="49"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="138" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="139"/>
-      <c r="C20" s="140"/>
-      <c r="D20" s="140"/>
-      <c r="E20" s="141"/>
-      <c r="F20" s="142"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="143"/>
-      <c r="J20" s="141"/>
-      <c r="K20" s="144"/>
-      <c r="L20" s="141"/>
-      <c r="M20" s="145" t="n">
+      <c r="X20" s="46"/>
+      <c r="Y20" s="46"/>
+      <c r="Z20" s="46"/>
+      <c r="AA20" s="46"/>
+      <c r="AB20" s="46"/>
+      <c r="AC20" s="46"/>
+      <c r="AD20" s="46"/>
+      <c r="AE20" s="46"/>
+      <c r="AF20" s="46"/>
+      <c r="AG20" s="46"/>
+      <c r="AH20" s="46"/>
+      <c r="AI20" s="46"/>
+      <c r="AJ20" s="145"/>
+      <c r="AK20" s="46"/>
+      <c r="AL20" s="46"/>
+      <c r="AM20" s="49"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="146" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="147"/>
+      <c r="C21" s="148"/>
+      <c r="D21" s="148"/>
+      <c r="E21" s="148"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
+      <c r="H21" s="149"/>
+      <c r="I21" s="124"/>
+      <c r="J21" s="150"/>
+      <c r="K21" s="150"/>
+      <c r="L21" s="150"/>
+      <c r="M21" s="149"/>
+      <c r="N21" s="151"/>
+      <c r="O21" s="149"/>
+      <c r="P21" s="152" t="n">
         <v>1.35</v>
       </c>
-      <c r="N20" s="146"/>
-      <c r="O20" s="147"/>
-      <c r="P20" s="147"/>
-      <c r="Q20" s="142"/>
-      <c r="R20" s="141"/>
-      <c r="S20" s="141" t="n">
+      <c r="Q21" s="153"/>
+      <c r="R21" s="154"/>
+      <c r="S21" s="154"/>
+      <c r="T21" s="124"/>
+      <c r="U21" s="149"/>
+      <c r="V21" s="149" t="n">
         <v>0.944</v>
       </c>
-      <c r="T20" s="148" t="n">
+      <c r="W21" s="155" t="n">
         <f aca="false">0.944/2</f>
         <v>0.472</v>
       </c>
-      <c r="U20" s="141"/>
-      <c r="V20" s="141"/>
-      <c r="W20" s="141"/>
-      <c r="X20" s="141"/>
-      <c r="Y20" s="141"/>
-      <c r="Z20" s="141"/>
-      <c r="AA20" s="141"/>
-      <c r="AB20" s="141"/>
-      <c r="AC20" s="141"/>
-      <c r="AD20" s="141"/>
-      <c r="AE20" s="141"/>
-      <c r="AF20" s="141"/>
-      <c r="AG20" s="149"/>
-      <c r="AH20" s="141"/>
-      <c r="AI20" s="141"/>
-      <c r="AJ20" s="150"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="151"/>
-      <c r="M21" s="131"/>
-      <c r="N21" s="131"/>
-      <c r="O21" s="152"/>
-      <c r="P21" s="131"/>
-      <c r="Q21" s="131"/>
-      <c r="R21" s="41"/>
-      <c r="S21" s="41"/>
-      <c r="T21" s="41"/>
-      <c r="U21" s="41"/>
-      <c r="V21" s="41"/>
-      <c r="W21" s="41"/>
-      <c r="AH21" s="41"/>
-      <c r="AI21" s="41"/>
-      <c r="AJ21" s="41"/>
+      <c r="X21" s="149"/>
+      <c r="Y21" s="149"/>
+      <c r="Z21" s="149"/>
+      <c r="AA21" s="149"/>
+      <c r="AB21" s="149"/>
+      <c r="AC21" s="149"/>
+      <c r="AD21" s="149"/>
+      <c r="AE21" s="149"/>
+      <c r="AF21" s="149"/>
+      <c r="AG21" s="149"/>
+      <c r="AH21" s="149"/>
+      <c r="AI21" s="149"/>
+      <c r="AJ21" s="156"/>
+      <c r="AK21" s="149"/>
+      <c r="AL21" s="149"/>
+      <c r="AM21" s="157"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="0"/>
-      <c r="M22" s="131"/>
-      <c r="N22" s="131"/>
-      <c r="O22" s="152"/>
-      <c r="P22" s="153"/>
-      <c r="Q22" s="153"/>
-      <c r="W22" s="0"/>
-      <c r="X22" s="0"/>
-      <c r="Y22" s="0"/>
-      <c r="Z22" s="0"/>
-      <c r="AA22" s="0"/>
-      <c r="AH22" s="41"/>
-      <c r="AI22" s="41"/>
-      <c r="AJ22" s="41"/>
+      <c r="I22" s="158"/>
+      <c r="P22" s="139"/>
+      <c r="Q22" s="139"/>
+      <c r="R22" s="159"/>
+      <c r="S22" s="139"/>
+      <c r="T22" s="139"/>
+      <c r="U22" s="41"/>
+      <c r="V22" s="41"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="41"/>
+      <c r="Z22" s="41"/>
+      <c r="AK22" s="41"/>
+      <c r="AL22" s="41"/>
+      <c r="AM22" s="41"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="0"/>
-      <c r="M23" s="131"/>
-      <c r="N23" s="131"/>
-      <c r="O23" s="152"/>
-      <c r="P23" s="131"/>
-      <c r="Q23" s="131"/>
-      <c r="W23" s="41"/>
-      <c r="AH23" s="41"/>
-      <c r="AI23" s="41"/>
-      <c r="AJ23" s="41"/>
+      <c r="A23" s="160"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="161"/>
+      <c r="D23" s="34"/>
+      <c r="I23" s="0"/>
+      <c r="P23" s="139"/>
+      <c r="Q23" s="139"/>
+      <c r="R23" s="159"/>
+      <c r="S23" s="162"/>
+      <c r="T23" s="162"/>
+      <c r="Z23" s="0"/>
+      <c r="AA23" s="0"/>
+      <c r="AB23" s="0"/>
+      <c r="AC23" s="0"/>
+      <c r="AD23" s="0"/>
+      <c r="AK23" s="41"/>
+      <c r="AL23" s="41"/>
+      <c r="AM23" s="41"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="B24" s="154"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="0"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="156"/>
-      <c r="N24" s="156"/>
-      <c r="O24" s="152"/>
-      <c r="P24" s="156"/>
-      <c r="Q24" s="156"/>
-      <c r="R24" s="41"/>
-      <c r="S24" s="41"/>
-      <c r="T24" s="41"/>
-      <c r="U24" s="41"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="41"/>
-      <c r="Y24" s="41"/>
+      <c r="I24" s="0"/>
+      <c r="P24" s="139"/>
+      <c r="Q24" s="139"/>
+      <c r="R24" s="159"/>
+      <c r="S24" s="139"/>
+      <c r="T24" s="139"/>
       <c r="Z24" s="41"/>
-      <c r="AA24" s="41"/>
-      <c r="AB24" s="41"/>
-      <c r="AC24" s="41"/>
-      <c r="AD24" s="41"/>
-      <c r="AE24" s="41"/>
-      <c r="AF24" s="41"/>
-      <c r="AG24" s="41"/>
-      <c r="AH24" s="41"/>
-      <c r="AI24" s="41"/>
-      <c r="AJ24" s="41"/>
+      <c r="AK24" s="41"/>
+      <c r="AL24" s="41"/>
+      <c r="AM24" s="41"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="0"/>
-      <c r="O25" s="152"/>
+      <c r="A25" s="0"/>
+      <c r="B25" s="163"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="164"/>
+      <c r="E25" s="164"/>
+      <c r="F25" s="164"/>
+      <c r="G25" s="164"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="0"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="165"/>
+      <c r="Q25" s="165"/>
+      <c r="R25" s="159"/>
+      <c r="S25" s="165"/>
+      <c r="T25" s="165"/>
+      <c r="U25" s="41"/>
+      <c r="V25" s="41"/>
       <c r="W25" s="41"/>
       <c r="X25" s="41"/>
-      <c r="Y25" s="157"/>
-      <c r="Z25" s="157"/>
-      <c r="AA25" s="157"/>
-      <c r="AB25" s="157"/>
-      <c r="AC25" s="157"/>
-      <c r="AD25" s="157"/>
-      <c r="AE25" s="157"/>
-      <c r="AF25" s="157"/>
-      <c r="AG25" s="157"/>
+      <c r="Y25" s="41"/>
+      <c r="Z25" s="41"/>
+      <c r="AA25" s="41"/>
+      <c r="AB25" s="41"/>
+      <c r="AC25" s="41"/>
+      <c r="AD25" s="41"/>
+      <c r="AE25" s="41"/>
+      <c r="AF25" s="41"/>
+      <c r="AG25" s="41"/>
       <c r="AH25" s="41"/>
       <c r="AI25" s="41"/>
       <c r="AJ25" s="41"/>
+      <c r="AK25" s="41"/>
+      <c r="AL25" s="41"/>
+      <c r="AM25" s="41"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="F26" s="0"/>
-      <c r="O26" s="152"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="41"/>
-      <c r="Y26" s="41"/>
+      <c r="I26" s="0"/>
+      <c r="R26" s="159"/>
       <c r="Z26" s="41"/>
       <c r="AA26" s="41"/>
-      <c r="AB26" s="41"/>
-      <c r="AC26" s="41"/>
-      <c r="AD26" s="41"/>
-      <c r="AE26" s="41"/>
-      <c r="AF26" s="41"/>
-      <c r="AG26" s="41"/>
-      <c r="AH26" s="41"/>
-      <c r="AI26" s="41"/>
-      <c r="AJ26" s="41"/>
+      <c r="AB26" s="166"/>
+      <c r="AC26" s="166"/>
+      <c r="AD26" s="166"/>
+      <c r="AE26" s="166"/>
+      <c r="AF26" s="166"/>
+      <c r="AG26" s="166"/>
+      <c r="AH26" s="166"/>
+      <c r="AI26" s="166"/>
+      <c r="AJ26" s="166"/>
+      <c r="AK26" s="41"/>
+      <c r="AL26" s="41"/>
+      <c r="AM26" s="41"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="0"/>
-      <c r="O27" s="152"/>
-      <c r="W27" s="41"/>
-      <c r="X27" s="41"/>
-      <c r="Y27" s="41"/>
+      <c r="A27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="R27" s="159"/>
       <c r="Z27" s="41"/>
       <c r="AA27" s="41"/>
       <c r="AB27" s="41"/>
@@ -3292,13 +3543,13 @@
       <c r="AH27" s="41"/>
       <c r="AI27" s="41"/>
       <c r="AJ27" s="41"/>
+      <c r="AK27" s="41"/>
+      <c r="AL27" s="41"/>
+      <c r="AM27" s="41"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="0"/>
-      <c r="O28" s="152"/>
-      <c r="W28" s="41"/>
-      <c r="X28" s="41"/>
-      <c r="Y28" s="41"/>
+      <c r="I28" s="0"/>
+      <c r="R28" s="159"/>
       <c r="Z28" s="41"/>
       <c r="AA28" s="41"/>
       <c r="AB28" s="41"/>
@@ -3310,12 +3561,13 @@
       <c r="AH28" s="41"/>
       <c r="AI28" s="41"/>
       <c r="AJ28" s="41"/>
+      <c r="AK28" s="41"/>
+      <c r="AL28" s="41"/>
+      <c r="AM28" s="41"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="0"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="41"/>
-      <c r="Y29" s="41"/>
+      <c r="I29" s="0"/>
+      <c r="R29" s="159"/>
       <c r="Z29" s="41"/>
       <c r="AA29" s="41"/>
       <c r="AB29" s="41"/>
@@ -3327,12 +3579,12 @@
       <c r="AH29" s="41"/>
       <c r="AI29" s="41"/>
       <c r="AJ29" s="41"/>
+      <c r="AK29" s="41"/>
+      <c r="AL29" s="41"/>
+      <c r="AM29" s="41"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="0"/>
-      <c r="W30" s="41"/>
-      <c r="X30" s="41"/>
-      <c r="Y30" s="41"/>
+      <c r="I30" s="0"/>
       <c r="Z30" s="41"/>
       <c r="AA30" s="41"/>
       <c r="AB30" s="41"/>
@@ -3344,12 +3596,12 @@
       <c r="AH30" s="41"/>
       <c r="AI30" s="41"/>
       <c r="AJ30" s="41"/>
+      <c r="AK30" s="41"/>
+      <c r="AL30" s="41"/>
+      <c r="AM30" s="41"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="0"/>
-      <c r="W31" s="41"/>
-      <c r="X31" s="41"/>
-      <c r="Y31" s="41"/>
+      <c r="I31" s="0"/>
       <c r="Z31" s="41"/>
       <c r="AA31" s="41"/>
       <c r="AB31" s="41"/>
@@ -3361,12 +3613,12 @@
       <c r="AH31" s="41"/>
       <c r="AI31" s="41"/>
       <c r="AJ31" s="41"/>
+      <c r="AK31" s="41"/>
+      <c r="AL31" s="41"/>
+      <c r="AM31" s="41"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="0"/>
-      <c r="W32" s="41"/>
-      <c r="X32" s="41"/>
-      <c r="Y32" s="41"/>
+      <c r="I32" s="0"/>
       <c r="Z32" s="41"/>
       <c r="AA32" s="41"/>
       <c r="AB32" s="41"/>
@@ -3378,11 +3630,12 @@
       <c r="AH32" s="41"/>
       <c r="AI32" s="41"/>
       <c r="AJ32" s="41"/>
+      <c r="AK32" s="41"/>
+      <c r="AL32" s="41"/>
+      <c r="AM32" s="41"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="0"/>
-      <c r="X33" s="41"/>
-      <c r="Y33" s="41"/>
+      <c r="I33" s="0"/>
       <c r="Z33" s="41"/>
       <c r="AA33" s="41"/>
       <c r="AB33" s="41"/>
@@ -3391,12 +3644,15 @@
       <c r="AE33" s="41"/>
       <c r="AF33" s="41"/>
       <c r="AG33" s="41"/>
+      <c r="AH33" s="41"/>
+      <c r="AI33" s="41"/>
+      <c r="AJ33" s="41"/>
+      <c r="AK33" s="41"/>
+      <c r="AL33" s="41"/>
+      <c r="AM33" s="41"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="0"/>
-      <c r="X34" s="41"/>
-      <c r="Y34" s="158"/>
-      <c r="Z34" s="41"/>
+      <c r="I34" s="0"/>
       <c r="AA34" s="41"/>
       <c r="AB34" s="41"/>
       <c r="AC34" s="41"/>
@@ -3404,36 +3660,37 @@
       <c r="AE34" s="41"/>
       <c r="AF34" s="41"/>
       <c r="AG34" s="41"/>
+      <c r="AH34" s="41"/>
+      <c r="AI34" s="41"/>
+      <c r="AJ34" s="41"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F35" s="0"/>
-      <c r="X35" s="41"/>
-      <c r="Y35" s="158"/>
-      <c r="Z35" s="41"/>
+      <c r="I35" s="0"/>
       <c r="AA35" s="41"/>
-      <c r="AB35" s="41"/>
+      <c r="AB35" s="167"/>
       <c r="AC35" s="41"/>
       <c r="AD35" s="41"/>
       <c r="AE35" s="41"/>
       <c r="AF35" s="41"/>
       <c r="AG35" s="41"/>
+      <c r="AH35" s="41"/>
+      <c r="AI35" s="41"/>
+      <c r="AJ35" s="41"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="X36" s="41"/>
-      <c r="Y36" s="41"/>
-      <c r="Z36" s="41"/>
+      <c r="I36" s="0"/>
       <c r="AA36" s="41"/>
-      <c r="AB36" s="41"/>
+      <c r="AB36" s="167"/>
       <c r="AC36" s="41"/>
       <c r="AD36" s="41"/>
       <c r="AE36" s="41"/>
       <c r="AF36" s="41"/>
       <c r="AG36" s="41"/>
+      <c r="AH36" s="41"/>
+      <c r="AI36" s="41"/>
+      <c r="AJ36" s="41"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="X37" s="41"/>
-      <c r="Y37" s="41"/>
-      <c r="Z37" s="41"/>
       <c r="AA37" s="41"/>
       <c r="AB37" s="41"/>
       <c r="AC37" s="41"/>
@@ -3441,11 +3698,11 @@
       <c r="AE37" s="41"/>
       <c r="AF37" s="41"/>
       <c r="AG37" s="41"/>
+      <c r="AH37" s="41"/>
+      <c r="AI37" s="41"/>
+      <c r="AJ37" s="41"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="X38" s="41"/>
-      <c r="Y38" s="41"/>
-      <c r="Z38" s="41"/>
       <c r="AA38" s="41"/>
       <c r="AB38" s="41"/>
       <c r="AC38" s="41"/>
@@ -3453,11 +3710,11 @@
       <c r="AE38" s="41"/>
       <c r="AF38" s="41"/>
       <c r="AG38" s="41"/>
+      <c r="AH38" s="41"/>
+      <c r="AI38" s="41"/>
+      <c r="AJ38" s="41"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="X39" s="41"/>
-      <c r="Y39" s="41"/>
-      <c r="Z39" s="41"/>
       <c r="AA39" s="41"/>
       <c r="AB39" s="41"/>
       <c r="AC39" s="41"/>
@@ -3465,11 +3722,11 @@
       <c r="AE39" s="41"/>
       <c r="AF39" s="41"/>
       <c r="AG39" s="41"/>
+      <c r="AH39" s="41"/>
+      <c r="AI39" s="41"/>
+      <c r="AJ39" s="41"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="X40" s="41"/>
-      <c r="Y40" s="41"/>
-      <c r="Z40" s="41"/>
       <c r="AA40" s="41"/>
       <c r="AB40" s="41"/>
       <c r="AC40" s="41"/>
@@ -3477,12 +3734,24 @@
       <c r="AE40" s="41"/>
       <c r="AF40" s="41"/>
       <c r="AG40" s="41"/>
+      <c r="AH40" s="41"/>
+      <c r="AI40" s="41"/>
+      <c r="AJ40" s="41"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA41" s="41"/>
+      <c r="AB41" s="41"/>
+      <c r="AC41" s="41"/>
+      <c r="AD41" s="41"/>
+      <c r="AE41" s="41"/>
+      <c r="AF41" s="41"/>
+      <c r="AG41" s="41"/>
+      <c r="AH41" s="41"/>
+      <c r="AI41" s="41"/>
+      <c r="AJ41" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
     <mergeCell ref="Z2:Z3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="AB2:AB3"/>
@@ -3494,9 +3763,9 @@
     <mergeCell ref="AH2:AH3"/>
     <mergeCell ref="AI2:AI3"/>
     <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="W4:W5"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="Y4:Y5"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AM2:AM3"/>
     <mergeCell ref="Z4:Z5"/>
     <mergeCell ref="AA4:AA5"/>
     <mergeCell ref="AB4:AB5"/>
@@ -3505,11 +3774,11 @@
     <mergeCell ref="AE4:AE5"/>
     <mergeCell ref="AF4:AF5"/>
     <mergeCell ref="AG4:AG5"/>
+    <mergeCell ref="AH4:AH5"/>
     <mergeCell ref="AI4:AI5"/>
     <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="AL4:AL5"/>
+    <mergeCell ref="AM4:AM5"/>
     <mergeCell ref="Z7:Z8"/>
     <mergeCell ref="AA7:AA8"/>
     <mergeCell ref="AB7:AB8"/>
@@ -3521,27 +3790,27 @@
     <mergeCell ref="AH7:AH8"/>
     <mergeCell ref="AI7:AI8"/>
     <mergeCell ref="AJ7:AJ8"/>
-    <mergeCell ref="AB9:AB10"/>
-    <mergeCell ref="AC9:AC10"/>
-    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AK7:AK8"/>
+    <mergeCell ref="AL7:AL8"/>
+    <mergeCell ref="AM7:AM8"/>
     <mergeCell ref="AE9:AE10"/>
     <mergeCell ref="AF9:AF10"/>
     <mergeCell ref="AG9:AG10"/>
     <mergeCell ref="AH9:AH10"/>
     <mergeCell ref="AI9:AI10"/>
     <mergeCell ref="AJ9:AJ10"/>
-    <mergeCell ref="AB13:AB14"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AL9:AL10"/>
+    <mergeCell ref="AM9:AM10"/>
     <mergeCell ref="AE13:AE14"/>
     <mergeCell ref="AF13:AF14"/>
     <mergeCell ref="AG13:AG14"/>
     <mergeCell ref="AH13:AH14"/>
     <mergeCell ref="AI13:AI14"/>
     <mergeCell ref="AJ13:AJ14"/>
-    <mergeCell ref="W15:W16"/>
-    <mergeCell ref="X15:X16"/>
-    <mergeCell ref="Y15:Y16"/>
+    <mergeCell ref="AK13:AK14"/>
+    <mergeCell ref="AL13:AL14"/>
+    <mergeCell ref="AM13:AM14"/>
     <mergeCell ref="Z15:Z16"/>
     <mergeCell ref="AA15:AA16"/>
     <mergeCell ref="AB15:AB16"/>
@@ -3553,6 +3822,9 @@
     <mergeCell ref="AH15:AH16"/>
     <mergeCell ref="AI15:AI16"/>
     <mergeCell ref="AJ15:AJ16"/>
+    <mergeCell ref="AK15:AK16"/>
+    <mergeCell ref="AL15:AL16"/>
+    <mergeCell ref="AM15:AM16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
change the name from concat to conc
</commit_message>
<xml_diff>
--- a/cells_initial_information/Data2.xlsx
+++ b/cells_initial_information/Data2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t xml:space="preserve">cell_name</t>
   </si>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">(-35.92; -391.47; -431.60)</t>
   </si>
   <si>
-    <t xml:space="preserve">2017_07_06_C_3_4</t>
+    <t xml:space="preserve">2017_07_06_C_3-4</t>
   </si>
   <si>
     <t xml:space="preserve">c112</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">c69</t>
   </si>
   <si>
-    <t xml:space="preserve">2017_07_06_C_4_3</t>
+    <t xml:space="preserve">2017_07_06_C_4-3</t>
   </si>
   <si>
     <t xml:space="preserve">c301</t>
@@ -215,6 +215,15 @@
   </si>
   <si>
     <t xml:space="preserve">human_spine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_03_04_A_6-7(0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_05_08_A_4-5(0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017_05_08_A_5-4(0)</t>
   </si>
 </sst>
 </file>
@@ -225,7 +234,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -379,21 +388,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFBFBFBF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -716,7 +710,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="164">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1367,22 +1361,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1469,7 +1447,7 @@
   <dimension ref="A1:BB41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19:D20"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3461,109 +3439,529 @@
       <c r="AM23" s="41"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I24" s="0"/>
-      <c r="P24" s="139"/>
-      <c r="Q24" s="139"/>
-      <c r="R24" s="159"/>
-      <c r="S24" s="139"/>
-      <c r="T24" s="139"/>
-      <c r="Z24" s="41"/>
-      <c r="AK24" s="41"/>
-      <c r="AL24" s="41"/>
-      <c r="AM24" s="41"/>
+      <c r="A24" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="65" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" s="68" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="I24" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="69" t="n">
+        <v>924.01</v>
+      </c>
+      <c r="K24" s="69" t="n">
+        <v>333.54</v>
+      </c>
+      <c r="L24" s="69" t="n">
+        <v>-257.4</v>
+      </c>
+      <c r="M24" s="69" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="N24" s="70" t="n">
+        <v>199</v>
+      </c>
+      <c r="O24" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="P24" s="68" t="n">
+        <v>0.763</v>
+      </c>
+      <c r="Q24" s="68" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="R24" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="S24" s="68" t="n">
+        <v>0.08501695029</v>
+      </c>
+      <c r="T24" s="68" t="n">
+        <v>0.0745871871</v>
+      </c>
+      <c r="U24" s="68" t="n">
+        <v>0.01042976319</v>
+      </c>
+      <c r="V24" s="68"/>
+      <c r="W24" s="68"/>
+      <c r="X24" s="68"/>
+      <c r="Y24" s="73" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="Z24" s="74" t="n">
+        <v>1.85989007744307</v>
+      </c>
+      <c r="AA24" s="74" t="n">
+        <v>0.324348142228853</v>
+      </c>
+      <c r="AB24" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC24" s="74" t="n">
+        <v>0.805034067065075</v>
+      </c>
+      <c r="AD24" s="74" t="n">
+        <v>0.290119432876338</v>
+      </c>
+      <c r="AE24" s="75" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF24" s="75" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG24" s="75" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AH24" s="75" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AI24" s="75" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AJ24" s="76" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AK24" s="77" t="n">
+        <v>200</v>
+      </c>
+      <c r="AL24" s="75" t="n">
+        <v>26</v>
+      </c>
+      <c r="AM24" s="78" t="n">
+        <v>225</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="163"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="164"/>
-      <c r="E25" s="164"/>
-      <c r="F25" s="164"/>
-      <c r="G25" s="164"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="0"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="165"/>
-      <c r="Q25" s="165"/>
-      <c r="R25" s="159"/>
-      <c r="S25" s="165"/>
-      <c r="T25" s="165"/>
-      <c r="U25" s="41"/>
-      <c r="V25" s="41"/>
-      <c r="W25" s="41"/>
-      <c r="X25" s="41"/>
-      <c r="Y25" s="41"/>
-      <c r="Z25" s="41"/>
-      <c r="AA25" s="41"/>
-      <c r="AB25" s="41"/>
-      <c r="AC25" s="41"/>
-      <c r="AD25" s="41"/>
-      <c r="AE25" s="41"/>
-      <c r="AF25" s="41"/>
-      <c r="AG25" s="41"/>
-      <c r="AH25" s="41"/>
-      <c r="AI25" s="41"/>
-      <c r="AJ25" s="41"/>
-      <c r="AK25" s="41"/>
-      <c r="AL25" s="41"/>
-      <c r="AM25" s="41"/>
+      <c r="A25" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="65" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="H25" s="68" t="n">
+        <v>50.6</v>
+      </c>
+      <c r="I25" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" s="69" t="n">
+        <v>873.38</v>
+      </c>
+      <c r="K25" s="69" t="n">
+        <v>331.97</v>
+      </c>
+      <c r="L25" s="69" t="n">
+        <v>-289.32</v>
+      </c>
+      <c r="M25" s="69" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="N25" s="70" t="n">
+        <v>3806</v>
+      </c>
+      <c r="O25" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="P25" s="68" t="n">
+        <v>0.905</v>
+      </c>
+      <c r="Q25" s="68" t="n">
+        <v>0.085</v>
+      </c>
+      <c r="R25" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="S25" s="68" t="n">
+        <v>0.0783942101</v>
+      </c>
+      <c r="T25" s="68" t="n">
+        <v>0.06459193692</v>
+      </c>
+      <c r="U25" s="68" t="n">
+        <v>0.01380227318</v>
+      </c>
+      <c r="V25" s="68"/>
+      <c r="W25" s="68"/>
+      <c r="X25" s="68"/>
+      <c r="Y25" s="73" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="Z25" s="75" t="n">
+        <v>1.85989007744307</v>
+      </c>
+      <c r="AA25" s="78" t="n">
+        <v>0.324348142228853</v>
+      </c>
+      <c r="AB25" s="75" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC25" s="75" t="n">
+        <v>0.805034067065075</v>
+      </c>
+      <c r="AD25" s="75" t="n">
+        <v>0.290119432876338</v>
+      </c>
+      <c r="AE25" s="75"/>
+      <c r="AF25" s="75"/>
+      <c r="AG25" s="75"/>
+      <c r="AH25" s="75"/>
+      <c r="AI25" s="75"/>
+      <c r="AJ25" s="76"/>
+      <c r="AK25" s="77"/>
+      <c r="AL25" s="75"/>
+      <c r="AM25" s="78"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I26" s="0"/>
-      <c r="R26" s="159"/>
-      <c r="Z26" s="41"/>
-      <c r="AA26" s="41"/>
-      <c r="AB26" s="166"/>
-      <c r="AC26" s="166"/>
-      <c r="AD26" s="166"/>
-      <c r="AE26" s="166"/>
-      <c r="AF26" s="166"/>
-      <c r="AG26" s="166"/>
-      <c r="AH26" s="166"/>
-      <c r="AI26" s="166"/>
-      <c r="AJ26" s="166"/>
-      <c r="AK26" s="41"/>
-      <c r="AL26" s="41"/>
-      <c r="AM26" s="41"/>
+      <c r="A26" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="84" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" s="85" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="86" t="n">
+        <v>91</v>
+      </c>
+      <c r="E26" s="86" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" s="86" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="86" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" s="87" t="n">
+        <v>83.8</v>
+      </c>
+      <c r="I26" s="87" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" s="88" t="n">
+        <v>-5.56</v>
+      </c>
+      <c r="K26" s="88" t="n">
+        <v>-325.88</v>
+      </c>
+      <c r="L26" s="89" t="n">
+        <v>-451.42</v>
+      </c>
+      <c r="M26" s="90" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="N26" s="91" t="n">
+        <v>82</v>
+      </c>
+      <c r="O26" s="92"/>
+      <c r="P26" s="87" t="n">
+        <v>0.782</v>
+      </c>
+      <c r="Q26" s="87" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="R26" s="87" t="n">
+        <v>11</v>
+      </c>
+      <c r="S26" s="87" t="n">
+        <v>0.16884774101</v>
+      </c>
+      <c r="T26" s="87" t="n">
+        <v>0.13906972096</v>
+      </c>
+      <c r="U26" s="87" t="n">
+        <v>0.02977802005</v>
+      </c>
+      <c r="V26" s="87"/>
+      <c r="W26" s="87"/>
+      <c r="X26" s="87"/>
+      <c r="Y26" s="0"/>
+      <c r="Z26" s="87" t="n">
+        <v>1.26083037757995</v>
+      </c>
+      <c r="AA26" s="93" t="n">
+        <v>0.417980287594169</v>
+      </c>
+      <c r="AB26" s="94" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC26" s="94" t="n">
+        <v>0.794059892657374</v>
+      </c>
+      <c r="AD26" s="94" t="n">
+        <v>0.67284340860646</v>
+      </c>
+      <c r="AE26" s="94" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF26" s="94" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG26" s="94" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AH26" s="94" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AI26" s="94" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AJ26" s="95" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AK26" s="96" t="n">
+        <v>275</v>
+      </c>
+      <c r="AL26" s="87" t="n">
+        <v>176</v>
+      </c>
+      <c r="AM26" s="93" t="n">
+        <v>450</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="I27" s="0"/>
-      <c r="R27" s="159"/>
-      <c r="Z27" s="41"/>
-      <c r="AA27" s="41"/>
-      <c r="AB27" s="41"/>
-      <c r="AC27" s="41"/>
-      <c r="AD27" s="41"/>
-      <c r="AE27" s="41"/>
-      <c r="AF27" s="41"/>
-      <c r="AG27" s="41"/>
-      <c r="AH27" s="41"/>
-      <c r="AI27" s="41"/>
-      <c r="AJ27" s="41"/>
-      <c r="AK27" s="41"/>
-      <c r="AL27" s="41"/>
-      <c r="AM27" s="41"/>
+      <c r="A27" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="99" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="100" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="101" t="n">
+        <v>42</v>
+      </c>
+      <c r="E27" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="H27" s="102" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="I27" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" s="103" t="n">
+        <v>-31.93</v>
+      </c>
+      <c r="K27" s="103" t="n">
+        <v>-355.4</v>
+      </c>
+      <c r="L27" s="103" t="n">
+        <v>-423.02</v>
+      </c>
+      <c r="M27" s="103" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="N27" s="104" t="n">
+        <v>4358</v>
+      </c>
+      <c r="O27" s="105" t="s">
+        <v>55</v>
+      </c>
+      <c r="P27" s="102" t="n">
+        <v>1.266</v>
+      </c>
+      <c r="Q27" s="102" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="R27" s="102" t="n">
+        <v>15</v>
+      </c>
+      <c r="S27" s="102" t="n">
+        <v>0.06818310193</v>
+      </c>
+      <c r="T27" s="102" t="n">
+        <v>0.03371715503</v>
+      </c>
+      <c r="U27" s="102" t="n">
+        <v>0.0344659469</v>
+      </c>
+      <c r="V27" s="102"/>
+      <c r="W27" s="102"/>
+      <c r="X27" s="102"/>
+      <c r="Y27" s="73" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="Z27" s="106" t="n">
+        <v>1.70290313569153</v>
+      </c>
+      <c r="AA27" s="106" t="n">
+        <v>0.33438126301574</v>
+      </c>
+      <c r="AB27" s="106" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC27" s="106" t="n">
+        <v>0.620744947626598</v>
+      </c>
+      <c r="AD27" s="106" t="n">
+        <v>0.173126100637382</v>
+      </c>
+      <c r="AE27" s="106" t="n">
+        <v>8</v>
+      </c>
+      <c r="AF27" s="106" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG27" s="106" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AH27" s="106" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AI27" s="106" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AJ27" s="107" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AK27" s="108" t="n">
+        <v>325</v>
+      </c>
+      <c r="AL27" s="106" t="n">
+        <v>126</v>
+      </c>
+      <c r="AM27" s="109" t="n">
+        <v>450</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I28" s="0"/>
-      <c r="R28" s="159"/>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="41"/>
-      <c r="AB28" s="41"/>
-      <c r="AC28" s="41"/>
-      <c r="AD28" s="41"/>
-      <c r="AE28" s="41"/>
-      <c r="AF28" s="41"/>
-      <c r="AG28" s="41"/>
-      <c r="AH28" s="41"/>
-      <c r="AI28" s="41"/>
-      <c r="AJ28" s="41"/>
-      <c r="AK28" s="41"/>
-      <c r="AL28" s="41"/>
-      <c r="AM28" s="41"/>
+      <c r="A28" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="99" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" s="100" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="101" t="n">
+        <v>68</v>
+      </c>
+      <c r="E28" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="H28" s="102" t="n">
+        <v>74.3</v>
+      </c>
+      <c r="I28" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" s="103" t="n">
+        <v>-35.92</v>
+      </c>
+      <c r="K28" s="103" t="n">
+        <v>-391.47</v>
+      </c>
+      <c r="L28" s="103" t="n">
+        <v>-431.6</v>
+      </c>
+      <c r="M28" s="103" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="N28" s="104" t="n">
+        <v>3923</v>
+      </c>
+      <c r="O28" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="P28" s="102" t="n">
+        <v>1.121</v>
+      </c>
+      <c r="Q28" s="102" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="R28" s="102" t="n">
+        <v>13</v>
+      </c>
+      <c r="S28" s="102" t="n">
+        <v>0.02865474235</v>
+      </c>
+      <c r="T28" s="102" t="n">
+        <v>0.01125841287</v>
+      </c>
+      <c r="U28" s="102" t="n">
+        <v>0.01739632948</v>
+      </c>
+      <c r="V28" s="102"/>
+      <c r="W28" s="102"/>
+      <c r="X28" s="102"/>
+      <c r="Y28" s="73" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="Z28" s="106" t="n">
+        <v>1.70290313569153</v>
+      </c>
+      <c r="AA28" s="106" t="n">
+        <v>0.33438126301574</v>
+      </c>
+      <c r="AB28" s="106" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC28" s="106" t="n">
+        <v>0.620744947626598</v>
+      </c>
+      <c r="AD28" s="106" t="n">
+        <v>0.173126100637382</v>
+      </c>
+      <c r="AE28" s="106"/>
+      <c r="AF28" s="106"/>
+      <c r="AG28" s="106"/>
+      <c r="AH28" s="106"/>
+      <c r="AI28" s="106"/>
+      <c r="AJ28" s="107"/>
+      <c r="AK28" s="108"/>
+      <c r="AL28" s="106"/>
+      <c r="AM28" s="109"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I29" s="0"/>
@@ -3667,7 +4065,7 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I35" s="0"/>
       <c r="AA35" s="41"/>
-      <c r="AB35" s="167"/>
+      <c r="AB35" s="163"/>
       <c r="AC35" s="41"/>
       <c r="AD35" s="41"/>
       <c r="AE35" s="41"/>
@@ -3680,7 +4078,7 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I36" s="0"/>
       <c r="AA36" s="41"/>
-      <c r="AB36" s="167"/>
+      <c r="AB36" s="163"/>
       <c r="AC36" s="41"/>
       <c r="AD36" s="41"/>
       <c r="AE36" s="41"/>
@@ -3751,7 +4149,7 @@
       <c r="AJ41" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
+  <mergeCells count="91">
     <mergeCell ref="Z2:Z3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="AB2:AB3"/>
@@ -3825,6 +4223,24 @@
     <mergeCell ref="AK15:AK16"/>
     <mergeCell ref="AL15:AL16"/>
     <mergeCell ref="AM15:AM16"/>
+    <mergeCell ref="AE24:AE25"/>
+    <mergeCell ref="AF24:AF25"/>
+    <mergeCell ref="AG24:AG25"/>
+    <mergeCell ref="AH24:AH25"/>
+    <mergeCell ref="AI24:AI25"/>
+    <mergeCell ref="AJ24:AJ25"/>
+    <mergeCell ref="AK24:AK25"/>
+    <mergeCell ref="AL24:AL25"/>
+    <mergeCell ref="AM24:AM25"/>
+    <mergeCell ref="AE27:AE28"/>
+    <mergeCell ref="AF27:AF28"/>
+    <mergeCell ref="AG27:AG28"/>
+    <mergeCell ref="AH27:AH28"/>
+    <mergeCell ref="AI27:AI28"/>
+    <mergeCell ref="AJ27:AJ28"/>
+    <mergeCell ref="AK27:AK28"/>
+    <mergeCell ref="AL27:AL28"/>
+    <mergeCell ref="AM27:AM28"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
correct the x y z in Data2.xlsx
</commit_message>
<xml_diff>
--- a/cells_initial_information/Data2.xlsx
+++ b/cells_initial_information/Data2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t xml:space="preserve">cell_name</t>
   </si>
@@ -172,6 +172,9 @@
     <t xml:space="preserve">2016_08_30_A</t>
   </si>
   <si>
+    <t xml:space="preserve">(573.96; 1353.07; -235.40)</t>
+  </si>
+  <si>
     <t xml:space="preserve">2017_02_20_B</t>
   </si>
   <si>
@@ -193,9 +196,15 @@
     <t xml:space="preserve">2017_04_03_B</t>
   </si>
   <si>
+    <t xml:space="preserve">(-606.35; 503.26; -222.56)</t>
+  </si>
+  <si>
     <t xml:space="preserve">2017_05_08_A_4-5</t>
   </si>
   <si>
+    <t xml:space="preserve">(-5.56; -325.88; -451.42)</t>
+  </si>
+  <si>
     <t xml:space="preserve">2017_05_08_A_5-4</t>
   </si>
   <si>
@@ -218,6 +227,9 @@
   </si>
   <si>
     <t xml:space="preserve">c301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-32.37; 940.67; -159.95)</t>
   </si>
   <si>
     <t xml:space="preserve">mouse_spine</t>
@@ -255,7 +267,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -277,7 +288,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -285,14 +295,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -300,7 +308,6 @@
       <color rgb="FF81D41A"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -308,7 +315,6 @@
       <color rgb="FFFF972F"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -316,7 +322,6 @@
       <color rgb="FFFFA6A6"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -324,21 +329,18 @@
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -346,7 +348,6 @@
       <color rgb="FF729FCF"/>
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -354,14 +355,12 @@
       <color rgb="FF729FCF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF729FCF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -369,14 +368,12 @@
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -384,17 +381,15 @@
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +466,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
         <bgColor rgb="FFB2B2B2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -718,7 +719,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="177">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -979,6 +980,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1115,10 +1120,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1251,14 +1252,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="13" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1271,6 +1264,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1407,6 +1404,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="14" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="11" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1417,6 +1418,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1439,7 +1444,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFD4EA6B"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -1460,7 +1465,7 @@
       <rgbColor rgb="FFBDD7EE"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFD4EA6B"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -1502,8 +1507,8 @@
   </sheetPr>
   <dimension ref="A1:BF41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1520,7 +1525,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="7.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="2" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="30.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="21"/>
@@ -2166,14 +2173,24 @@
       <c r="I6" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
+      <c r="J6" s="38" t="n">
+        <v>573.96</v>
+      </c>
+      <c r="K6" s="38" t="n">
+        <v>1353.07</v>
+      </c>
+      <c r="L6" s="38" t="n">
+        <v>-235.4</v>
+      </c>
       <c r="M6" s="38" t="n">
         <v>0.031</v>
       </c>
-      <c r="N6" s="39"/>
-      <c r="O6" s="40"/>
+      <c r="N6" s="65" t="n">
+        <v>3532</v>
+      </c>
+      <c r="O6" s="65" t="s">
+        <v>50</v>
+      </c>
       <c r="P6" s="37" t="n">
         <v>0.644</v>
       </c>
@@ -2227,34 +2244,34 @@
       <c r="AE6" s="40" t="n">
         <v>0.190167451046957</v>
       </c>
-      <c r="AF6" s="65" t="n">
+      <c r="AF6" s="66" t="n">
         <v>4</v>
       </c>
-      <c r="AG6" s="65" t="n">
+      <c r="AG6" s="66" t="n">
         <v>0.569423206285454</v>
       </c>
-      <c r="AH6" s="65" t="n">
+      <c r="AH6" s="66" t="n">
         <v>0.204818840259996</v>
       </c>
-      <c r="AI6" s="65" t="n">
+      <c r="AI6" s="66" t="n">
         <v>3</v>
       </c>
-      <c r="AJ6" s="65" t="n">
+      <c r="AJ6" s="66" t="n">
         <v>16</v>
       </c>
-      <c r="AK6" s="65" t="n">
+      <c r="AK6" s="66" t="n">
         <v>0.4</v>
       </c>
-      <c r="AL6" s="65" t="n">
+      <c r="AL6" s="66" t="n">
         <v>0.8</v>
       </c>
-      <c r="AM6" s="65" t="n">
+      <c r="AM6" s="66" t="n">
         <v>0.1</v>
       </c>
       <c r="AN6" s="33" t="n">
         <v>0.4</v>
       </c>
-      <c r="AO6" s="66" t="n">
+      <c r="AO6" s="67" t="n">
         <v>300</v>
       </c>
       <c r="AP6" s="37" t="n">
@@ -2265,8 +2282,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="67" t="s">
-        <v>50</v>
+      <c r="A7" s="68" t="s">
+        <v>51</v>
       </c>
       <c r="B7" s="47" t="n">
         <v>6</v>
@@ -2380,7 +2397,7 @@
       <c r="AN7" s="60" t="n">
         <v>0.8</v>
       </c>
-      <c r="AO7" s="68" t="n">
+      <c r="AO7" s="69" t="n">
         <v>125</v>
       </c>
       <c r="AP7" s="57" t="n">
@@ -2391,8 +2408,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="67" t="s">
-        <v>50</v>
+      <c r="A8" s="68" t="s">
+        <v>51</v>
       </c>
       <c r="B8" s="47" t="n">
         <v>6</v>
@@ -2484,145 +2501,145 @@
       <c r="AL8" s="57"/>
       <c r="AM8" s="57"/>
       <c r="AN8" s="60"/>
-      <c r="AO8" s="68"/>
+      <c r="AO8" s="69"/>
       <c r="AP8" s="57"/>
       <c r="AQ8" s="58"/>
     </row>
-    <row r="9" s="86" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="70" t="n">
+    <row r="9" s="87" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="71" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="72" t="n">
+      <c r="C9" s="72" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="73" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" s="73" t="n">
+      <c r="F9" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="74" t="n">
         <v>32.6</v>
       </c>
-      <c r="I9" s="73" t="s">
+      <c r="I9" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="74" t="n">
+      <c r="J9" s="75" t="n">
         <v>924.01</v>
       </c>
-      <c r="K9" s="74" t="n">
+      <c r="K9" s="75" t="n">
         <v>333.54</v>
       </c>
-      <c r="L9" s="74" t="n">
+      <c r="L9" s="75" t="n">
         <v>-257.4</v>
       </c>
-      <c r="M9" s="74" t="n">
+      <c r="M9" s="75" t="n">
         <v>0.114</v>
       </c>
-      <c r="N9" s="75" t="n">
+      <c r="N9" s="76" t="n">
         <v>199</v>
       </c>
-      <c r="O9" s="76" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="73" t="n">
+      <c r="O9" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9" s="74" t="n">
         <v>0.763</v>
       </c>
-      <c r="Q9" s="73" t="n">
+      <c r="Q9" s="74" t="n">
         <v>0.134</v>
       </c>
-      <c r="R9" s="77" t="n">
+      <c r="R9" s="78" t="n">
         <v>1</v>
       </c>
-      <c r="S9" s="73" t="n">
+      <c r="S9" s="74" t="n">
         <v>0.08501695029</v>
       </c>
-      <c r="T9" s="73" t="n">
+      <c r="T9" s="74" t="n">
         <v>0.0745871871</v>
       </c>
-      <c r="U9" s="73" t="n">
+      <c r="U9" s="74" t="n">
         <v>0.01042976319</v>
       </c>
-      <c r="V9" s="78" t="n">
+      <c r="V9" s="79" t="n">
         <f aca="false">2*W9</f>
         <v>0.522262129884443</v>
       </c>
-      <c r="W9" s="73" t="n">
+      <c r="W9" s="74" t="n">
         <f aca="false">(3/4*T9/PI())^(1/3)</f>
         <v>0.261131064942221</v>
       </c>
-      <c r="X9" s="73" t="n">
+      <c r="X9" s="74" t="n">
         <f aca="false">4*PI()*W9^2</f>
         <v>0.856893688039415</v>
       </c>
-      <c r="Y9" s="73" t="n">
+      <c r="Y9" s="74" t="n">
         <f aca="false">(U9/(P9*PI()))^0.5*2*PI()*P9</f>
         <v>0.316230987973677</v>
       </c>
-      <c r="Z9" s="79" t="n">
+      <c r="Z9" s="80" t="n">
         <f aca="false">2*PI()*(Q9/2)*P9</f>
         <v>0.321202716088328</v>
       </c>
-      <c r="AA9" s="79" t="n">
+      <c r="AA9" s="80" t="n">
         <f aca="false">PI()*(Q9/2)^2*P9</f>
         <v>0.010760290988959</v>
       </c>
-      <c r="AB9" s="79" t="n">
+      <c r="AB9" s="80" t="n">
         <f aca="false">Z9+X9</f>
         <v>1.17809640412774</v>
       </c>
-      <c r="AC9" s="80" t="n">
+      <c r="AC9" s="81" t="n">
         <v>1.08</v>
       </c>
-      <c r="AD9" s="81" t="n">
+      <c r="AD9" s="82" t="n">
         <v>1.85989007744307</v>
       </c>
-      <c r="AE9" s="81" t="n">
+      <c r="AE9" s="82" t="n">
         <v>0.324348142228853</v>
       </c>
       <c r="AF9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="AG9" s="81" t="n">
+      <c r="AG9" s="82" t="n">
         <v>0.805034067065075</v>
       </c>
-      <c r="AH9" s="81" t="n">
+      <c r="AH9" s="82" t="n">
         <v>0.290119432876338</v>
       </c>
-      <c r="AI9" s="82" t="n">
+      <c r="AI9" s="83" t="n">
         <v>5</v>
       </c>
-      <c r="AJ9" s="82" t="n">
+      <c r="AJ9" s="83" t="n">
         <v>20</v>
       </c>
-      <c r="AK9" s="82" t="n">
+      <c r="AK9" s="83" t="n">
         <v>0.7</v>
       </c>
-      <c r="AL9" s="82" t="n">
+      <c r="AL9" s="83" t="n">
         <v>0.9</v>
       </c>
-      <c r="AM9" s="82" t="n">
+      <c r="AM9" s="83" t="n">
         <v>0.1</v>
       </c>
-      <c r="AN9" s="83" t="n">
+      <c r="AN9" s="84" t="n">
         <v>0.7</v>
       </c>
-      <c r="AO9" s="84" t="n">
+      <c r="AO9" s="85" t="n">
         <v>200</v>
       </c>
-      <c r="AP9" s="82" t="n">
+      <c r="AP9" s="83" t="n">
         <v>26</v>
       </c>
-      <c r="AQ9" s="85" t="n">
+      <c r="AQ9" s="86" t="n">
         <v>225</v>
       </c>
       <c r="AR9" s="0"/>
@@ -2641,125 +2658,125 @@
       <c r="BE9" s="0"/>
       <c r="BF9" s="0"/>
     </row>
-    <row r="10" s="86" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="70" t="n">
+    <row r="10" s="87" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="71" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="72" t="n">
+      <c r="C10" s="72" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="73" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="73" t="n">
+      <c r="F10" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="74" t="n">
         <v>50.6</v>
       </c>
-      <c r="I10" s="73" t="s">
+      <c r="I10" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="74" t="n">
+      <c r="J10" s="75" t="n">
         <v>873.38</v>
       </c>
-      <c r="K10" s="74" t="n">
+      <c r="K10" s="75" t="n">
         <v>331.97</v>
       </c>
-      <c r="L10" s="74" t="n">
+      <c r="L10" s="75" t="n">
         <v>-289.32</v>
       </c>
-      <c r="M10" s="74" t="n">
+      <c r="M10" s="75" t="n">
         <v>0.039</v>
       </c>
-      <c r="N10" s="75" t="n">
+      <c r="N10" s="76" t="n">
         <v>3806</v>
       </c>
-      <c r="O10" s="76" t="s">
-        <v>55</v>
-      </c>
-      <c r="P10" s="73" t="n">
+      <c r="O10" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="P10" s="74" t="n">
         <v>0.905</v>
       </c>
-      <c r="Q10" s="73" t="n">
+      <c r="Q10" s="74" t="n">
         <v>0.085</v>
       </c>
-      <c r="R10" s="77" t="n">
+      <c r="R10" s="78" t="n">
         <v>1</v>
       </c>
-      <c r="S10" s="73" t="n">
+      <c r="S10" s="74" t="n">
         <v>0.0783942101</v>
       </c>
-      <c r="T10" s="73" t="n">
+      <c r="T10" s="74" t="n">
         <v>0.06459193692</v>
       </c>
-      <c r="U10" s="73" t="n">
+      <c r="U10" s="74" t="n">
         <v>0.01380227318</v>
       </c>
-      <c r="V10" s="78" t="n">
+      <c r="V10" s="79" t="n">
         <f aca="false">2*W10</f>
         <v>0.497805734533224</v>
       </c>
-      <c r="W10" s="73" t="n">
+      <c r="W10" s="74" t="n">
         <f aca="false">(3/4*T10/PI())^(1/3)</f>
         <v>0.248902867266612</v>
       </c>
-      <c r="X10" s="73" t="n">
+      <c r="X10" s="74" t="n">
         <f aca="false">4*PI()*W10^2</f>
         <v>0.778519801270257</v>
       </c>
-      <c r="Y10" s="73" t="n">
+      <c r="Y10" s="74" t="n">
         <f aca="false">(U10/(P10*PI()))^0.5*2*PI()*P10</f>
         <v>0.396190931863617</v>
       </c>
-      <c r="Z10" s="79" t="n">
+      <c r="Z10" s="80" t="n">
         <f aca="false">2*PI()*(Q10/2)*P10</f>
         <v>0.241667014877395</v>
       </c>
-      <c r="AA10" s="79" t="n">
+      <c r="AA10" s="80" t="n">
         <f aca="false">PI()*(Q10/2)^2*P10</f>
         <v>0.00513542406614464</v>
       </c>
-      <c r="AB10" s="79" t="n">
+      <c r="AB10" s="80" t="n">
         <f aca="false">Z10+X10</f>
         <v>1.02018681614765</v>
       </c>
-      <c r="AC10" s="80" t="n">
+      <c r="AC10" s="81" t="n">
         <v>1.08</v>
       </c>
-      <c r="AD10" s="82" t="n">
+      <c r="AD10" s="83" t="n">
         <v>1.85989007744307</v>
       </c>
-      <c r="AE10" s="85" t="n">
+      <c r="AE10" s="86" t="n">
         <v>0.324348142228853</v>
       </c>
-      <c r="AF10" s="82" t="n">
+      <c r="AF10" s="83" t="n">
         <v>8</v>
       </c>
-      <c r="AG10" s="82" t="n">
+      <c r="AG10" s="83" t="n">
         <v>0.805034067065075</v>
       </c>
-      <c r="AH10" s="82" t="n">
+      <c r="AH10" s="83" t="n">
         <v>0.290119432876338</v>
       </c>
-      <c r="AI10" s="82"/>
-      <c r="AJ10" s="82"/>
-      <c r="AK10" s="82"/>
-      <c r="AL10" s="82"/>
-      <c r="AM10" s="82"/>
-      <c r="AN10" s="83"/>
-      <c r="AO10" s="84"/>
-      <c r="AP10" s="82"/>
-      <c r="AQ10" s="85"/>
+      <c r="AI10" s="83"/>
+      <c r="AJ10" s="83"/>
+      <c r="AK10" s="83"/>
+      <c r="AL10" s="83"/>
+      <c r="AM10" s="83"/>
+      <c r="AN10" s="84"/>
+      <c r="AO10" s="85"/>
+      <c r="AP10" s="83"/>
+      <c r="AQ10" s="86"/>
       <c r="AR10" s="0"/>
       <c r="AS10" s="0"/>
       <c r="AT10" s="0"/>
@@ -2777,13 +2794,13 @@
       <c r="BF10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="88" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="89" t="n">
+      <c r="A11" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="89" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="90" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="49" t="n">
@@ -2804,14 +2821,24 @@
       <c r="I11" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
+      <c r="J11" s="51" t="n">
+        <v>-606.35</v>
+      </c>
+      <c r="K11" s="51" t="n">
+        <v>503.26</v>
+      </c>
+      <c r="L11" s="51" t="n">
+        <v>-222.56</v>
+      </c>
       <c r="M11" s="51" t="n">
         <v>0.109</v>
       </c>
-      <c r="N11" s="52"/>
-      <c r="O11" s="53"/>
+      <c r="N11" s="65" t="n">
+        <v>4746</v>
+      </c>
+      <c r="O11" s="65" t="s">
+        <v>58</v>
+      </c>
       <c r="P11" s="50" t="n">
         <v>0.823</v>
       </c>
@@ -2903,80 +2930,82 @@
       </c>
     </row>
     <row r="12" s="106" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="90" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="91" t="n">
+      <c r="A12" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="92" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="92" t="n">
+      <c r="C12" s="93" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="93" t="n">
+      <c r="D12" s="94" t="n">
         <v>91</v>
       </c>
-      <c r="E12" s="93" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" s="93" t="n">
+      <c r="E12" s="94" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="94" t="n">
         <v>1</v>
       </c>
-      <c r="G12" s="93" t="n">
+      <c r="G12" s="94" t="n">
         <v>1</v>
       </c>
-      <c r="H12" s="94" t="n">
+      <c r="H12" s="95" t="n">
         <v>83.8</v>
       </c>
-      <c r="I12" s="94" t="s">
+      <c r="I12" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="95" t="n">
+      <c r="J12" s="96" t="n">
         <v>-5.56</v>
       </c>
-      <c r="K12" s="95" t="n">
+      <c r="K12" s="96" t="n">
         <v>-325.88</v>
       </c>
-      <c r="L12" s="96" t="n">
+      <c r="L12" s="97" t="n">
         <v>-451.42</v>
       </c>
-      <c r="M12" s="97" t="n">
+      <c r="M12" s="98" t="n">
         <v>0.14</v>
       </c>
-      <c r="N12" s="98" t="n">
+      <c r="N12" s="99" t="n">
         <v>82</v>
       </c>
-      <c r="O12" s="99"/>
-      <c r="P12" s="94" t="n">
+      <c r="O12" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12" s="95" t="n">
         <v>0.782</v>
       </c>
-      <c r="Q12" s="94" t="n">
+      <c r="Q12" s="95" t="n">
         <v>0.164</v>
       </c>
-      <c r="R12" s="94" t="n">
+      <c r="R12" s="95" t="n">
         <v>11</v>
       </c>
-      <c r="S12" s="94" t="n">
+      <c r="S12" s="95" t="n">
         <v>0.16884774101</v>
       </c>
-      <c r="T12" s="94" t="n">
+      <c r="T12" s="95" t="n">
         <v>0.13906972096</v>
       </c>
-      <c r="U12" s="94" t="n">
+      <c r="U12" s="95" t="n">
         <v>0.02977802005</v>
       </c>
       <c r="V12" s="100" t="n">
         <f aca="false">2*W12</f>
         <v>0.642803136179527</v>
       </c>
-      <c r="W12" s="94" t="n">
+      <c r="W12" s="95" t="n">
         <f aca="false">(3/4*T12/PI())^(1/3)</f>
         <v>0.321401568089763</v>
       </c>
-      <c r="X12" s="94" t="n">
+      <c r="X12" s="95" t="n">
         <f aca="false">4*PI()*W12^2</f>
         <v>1.29809311559886</v>
       </c>
-      <c r="Y12" s="94" t="n">
+      <c r="Y12" s="95" t="n">
         <f aca="false">(U12/(P12*PI()))^0.5*2*PI()*P12</f>
         <v>0.540948869522908</v>
       </c>
@@ -2993,7 +3022,7 @@
         <v>1.70099609023644</v>
       </c>
       <c r="AC12" s="0"/>
-      <c r="AD12" s="94" t="n">
+      <c r="AD12" s="95" t="n">
         <v>1.26083037757995</v>
       </c>
       <c r="AE12" s="102" t="n">
@@ -3029,7 +3058,7 @@
       <c r="AO12" s="105" t="n">
         <v>275</v>
       </c>
-      <c r="AP12" s="94" t="n">
+      <c r="AP12" s="95" t="n">
         <v>176</v>
       </c>
       <c r="AQ12" s="102" t="n">
@@ -3053,7 +3082,7 @@
     </row>
     <row r="13" s="121" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="107" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B13" s="108" t="n">
         <v>4</v>
@@ -3095,7 +3124,7 @@
         <v>4358</v>
       </c>
       <c r="O13" s="114" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P13" s="111" t="n">
         <v>1.266</v>
@@ -3143,7 +3172,7 @@
         <f aca="false">Z13+X13</f>
         <v>1.00187807403263</v>
       </c>
-      <c r="AC13" s="80" t="n">
+      <c r="AC13" s="81" t="n">
         <v>1.08</v>
       </c>
       <c r="AD13" s="117" t="n">
@@ -3206,7 +3235,7 @@
     </row>
     <row r="14" s="121" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="107" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B14" s="108" t="n">
         <v>4</v>
@@ -3248,7 +3277,7 @@
         <v>3923</v>
       </c>
       <c r="O14" s="114" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="P14" s="111" t="n">
         <v>1.121</v>
@@ -3296,7 +3325,7 @@
         <f aca="false">Z14+X14</f>
         <v>0.602139137880816</v>
       </c>
-      <c r="AC14" s="80" t="n">
+      <c r="AC14" s="81" t="n">
         <v>1.08</v>
       </c>
       <c r="AD14" s="117" t="n">
@@ -3341,7 +3370,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="122" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>5</v>
@@ -3350,7 +3379,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="123" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E15" s="123" t="n">
         <v>1</v>
@@ -3422,34 +3451,34 @@
         <v>0</v>
       </c>
       <c r="AC15" s="0"/>
-      <c r="AD15" s="65" t="n">
+      <c r="AD15" s="66" t="n">
         <v>0.148073219653408</v>
       </c>
       <c r="AE15" s="124" t="n">
         <v>0.144962080584371</v>
       </c>
-      <c r="AF15" s="65" t="n">
+      <c r="AF15" s="66" t="n">
         <v>6</v>
       </c>
-      <c r="AG15" s="65" t="n">
+      <c r="AG15" s="66" t="n">
         <v>0.14743558175711</v>
       </c>
-      <c r="AH15" s="65" t="n">
+      <c r="AH15" s="66" t="n">
         <v>0.166458165561462</v>
       </c>
-      <c r="AI15" s="65" t="n">
+      <c r="AI15" s="66" t="n">
         <v>4</v>
       </c>
-      <c r="AJ15" s="65" t="n">
+      <c r="AJ15" s="66" t="n">
         <v>19</v>
       </c>
-      <c r="AK15" s="65" t="n">
+      <c r="AK15" s="66" t="n">
         <v>0.1</v>
       </c>
-      <c r="AL15" s="65" t="n">
+      <c r="AL15" s="66" t="n">
         <v>0.5</v>
       </c>
-      <c r="AM15" s="65" t="n">
+      <c r="AM15" s="66" t="n">
         <v>0.1</v>
       </c>
       <c r="AN15" s="33" t="n">
@@ -3458,7 +3487,7 @@
       <c r="AO15" s="125" t="n">
         <v>225</v>
       </c>
-      <c r="AP15" s="65" t="n">
+      <c r="AP15" s="66" t="n">
         <v>51</v>
       </c>
       <c r="AQ15" s="124" t="n">
@@ -3467,7 +3496,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="126" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>5</v>
@@ -3476,7 +3505,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="123" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E16" s="123" t="n">
         <v>1</v>
@@ -3548,24 +3577,24 @@
         <v>0.77289342852701</v>
       </c>
       <c r="AC16" s="0"/>
-      <c r="AD16" s="65"/>
+      <c r="AD16" s="66"/>
       <c r="AE16" s="124"/>
-      <c r="AF16" s="65"/>
-      <c r="AG16" s="65"/>
-      <c r="AH16" s="65"/>
-      <c r="AI16" s="65"/>
-      <c r="AJ16" s="65"/>
-      <c r="AK16" s="65"/>
-      <c r="AL16" s="65"/>
-      <c r="AM16" s="65"/>
+      <c r="AF16" s="66"/>
+      <c r="AG16" s="66"/>
+      <c r="AH16" s="66"/>
+      <c r="AI16" s="66"/>
+      <c r="AJ16" s="66"/>
+      <c r="AK16" s="66"/>
+      <c r="AL16" s="66"/>
+      <c r="AM16" s="66"/>
       <c r="AN16" s="33"/>
       <c r="AO16" s="125"/>
-      <c r="AP16" s="65"/>
+      <c r="AP16" s="66"/>
       <c r="AQ16" s="124"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="127" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B17" s="128" t="n">
         <v>1</v>
@@ -3574,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="130" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E17" s="130" t="n">
         <v>2</v>
@@ -3591,14 +3620,24 @@
       <c r="I17" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="132"/>
-      <c r="K17" s="132"/>
-      <c r="L17" s="132"/>
+      <c r="J17" s="132" t="n">
+        <v>-32.37</v>
+      </c>
+      <c r="K17" s="132" t="n">
+        <v>940.67</v>
+      </c>
+      <c r="L17" s="132" t="n">
+        <v>-159.95</v>
+      </c>
       <c r="M17" s="132" t="n">
         <v>0.081</v>
       </c>
-      <c r="N17" s="133"/>
-      <c r="O17" s="134"/>
+      <c r="N17" s="65" t="n">
+        <v>5478</v>
+      </c>
+      <c r="O17" s="65" t="s">
+        <v>69</v>
+      </c>
       <c r="P17" s="131" t="n">
         <v>1.063</v>
       </c>
@@ -3617,7 +3656,7 @@
       <c r="U17" s="131" t="n">
         <v>0.02187695886</v>
       </c>
-      <c r="V17" s="135" t="n">
+      <c r="V17" s="133" t="n">
         <f aca="false">2*W17</f>
         <v>0.511890414376072</v>
       </c>
@@ -3633,59 +3672,59 @@
         <f aca="false">(U17/(P17*PI()))^0.5*2*PI()*P17</f>
         <v>0.540586305085219</v>
       </c>
-      <c r="Z17" s="136" t="n">
+      <c r="Z17" s="134" t="n">
         <f aca="false">2*PI()*(Q17/2)*P17</f>
         <v>0.390723019919616</v>
       </c>
-      <c r="AA17" s="136" t="n">
+      <c r="AA17" s="134" t="n">
         <f aca="false">PI()*(Q17/2)^2*P17</f>
         <v>0.0114286483326488</v>
       </c>
-      <c r="AB17" s="136" t="n">
+      <c r="AB17" s="134" t="n">
         <f aca="false">Z17+X17</f>
         <v>1.21392018627722</v>
       </c>
-      <c r="AC17" s="137"/>
+      <c r="AC17" s="135"/>
       <c r="AD17" s="131" t="n">
         <v>0.585780971744615</v>
       </c>
-      <c r="AE17" s="134" t="n">
+      <c r="AE17" s="136" t="n">
         <v>0.287981450721111</v>
       </c>
-      <c r="AF17" s="138" t="n">
+      <c r="AF17" s="137" t="n">
         <v>4</v>
       </c>
-      <c r="AG17" s="138" t="n">
+      <c r="AG17" s="137" t="n">
         <v>0.489876551485588</v>
       </c>
-      <c r="AH17" s="138" t="n">
+      <c r="AH17" s="137" t="n">
         <v>0.277535462267387</v>
       </c>
-      <c r="AI17" s="138" t="n">
+      <c r="AI17" s="137" t="n">
         <v>3</v>
       </c>
-      <c r="AJ17" s="138" t="n">
+      <c r="AJ17" s="137" t="n">
         <v>15</v>
       </c>
-      <c r="AK17" s="138" t="n">
+      <c r="AK17" s="137" t="n">
         <v>0.3</v>
       </c>
-      <c r="AL17" s="138" t="n">
+      <c r="AL17" s="137" t="n">
         <v>0.7</v>
       </c>
-      <c r="AM17" s="138" t="n">
+      <c r="AM17" s="137" t="n">
         <v>0.1</v>
       </c>
-      <c r="AN17" s="139" t="n">
+      <c r="AN17" s="138" t="n">
         <v>0.5</v>
       </c>
-      <c r="AO17" s="140" t="n">
+      <c r="AO17" s="139" t="n">
         <v>325</v>
       </c>
       <c r="AP17" s="131" t="n">
         <v>1</v>
       </c>
-      <c r="AQ17" s="134" t="n">
+      <c r="AQ17" s="136" t="n">
         <v>325</v>
       </c>
     </row>
@@ -3712,99 +3751,99 @@
       <c r="W18" s="0"/>
       <c r="X18" s="0"/>
       <c r="Y18" s="0"/>
-      <c r="Z18" s="136" t="n">
+      <c r="Z18" s="134" t="n">
         <f aca="false">2*PI()*(Q18/2)*P18</f>
         <v>0</v>
       </c>
       <c r="AA18" s="0"/>
-      <c r="AB18" s="136" t="n">
+      <c r="AB18" s="134" t="n">
         <f aca="false">Z18+X18</f>
         <v>0</v>
       </c>
-      <c r="AC18" s="141"/>
-      <c r="AD18" s="141"/>
-      <c r="AE18" s="141"/>
-      <c r="AF18" s="141"/>
-      <c r="AG18" s="141"/>
-      <c r="AH18" s="141"/>
-      <c r="AI18" s="141"/>
-      <c r="AJ18" s="141"/>
-      <c r="AK18" s="141"/>
-      <c r="AL18" s="141"/>
-      <c r="AM18" s="141"/>
-      <c r="AN18" s="141"/>
-      <c r="AO18" s="141"/>
-      <c r="AP18" s="141"/>
-      <c r="AQ18" s="142"/>
+      <c r="AC18" s="140"/>
+      <c r="AD18" s="140"/>
+      <c r="AE18" s="140"/>
+      <c r="AF18" s="140"/>
+      <c r="AG18" s="140"/>
+      <c r="AH18" s="140"/>
+      <c r="AI18" s="140"/>
+      <c r="AJ18" s="140"/>
+      <c r="AK18" s="140"/>
+      <c r="AL18" s="140"/>
+      <c r="AM18" s="140"/>
+      <c r="AN18" s="140"/>
+      <c r="AO18" s="140"/>
+      <c r="AP18" s="140"/>
+      <c r="AQ18" s="141"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="143" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="144"/>
+      <c r="A19" s="142" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="143"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
       <c r="G19" s="23"/>
-      <c r="J19" s="144"/>
-      <c r="K19" s="144"/>
-      <c r="L19" s="144"/>
-      <c r="N19" s="145"/>
-      <c r="P19" s="146" t="n">
+      <c r="J19" s="143"/>
+      <c r="K19" s="143"/>
+      <c r="L19" s="143"/>
+      <c r="N19" s="144"/>
+      <c r="P19" s="145" t="n">
         <v>0.73</v>
       </c>
-      <c r="Q19" s="147" t="n">
+      <c r="Q19" s="146" t="n">
         <v>0.25</v>
       </c>
-      <c r="R19" s="148"/>
-      <c r="S19" s="148"/>
+      <c r="R19" s="147"/>
+      <c r="S19" s="147"/>
       <c r="T19" s="0"/>
       <c r="U19" s="45"/>
       <c r="V19" s="45"/>
       <c r="W19" s="45"/>
-      <c r="X19" s="80" t="n">
+      <c r="X19" s="81" t="n">
         <v>0.37</v>
       </c>
-      <c r="Y19" s="80"/>
-      <c r="Z19" s="136" t="n">
+      <c r="Y19" s="81"/>
+      <c r="Z19" s="134" t="n">
         <f aca="false">2*PI()*(Q19/2)*P19</f>
         <v>0.573340659280137</v>
       </c>
-      <c r="AA19" s="80"/>
-      <c r="AB19" s="136" t="n">
+      <c r="AA19" s="81"/>
+      <c r="AB19" s="134" t="n">
         <f aca="false">Z19+X19</f>
         <v>0.943340659280137</v>
       </c>
-      <c r="AC19" s="80" t="n">
+      <c r="AC19" s="81" t="n">
         <v>1.08</v>
       </c>
       <c r="AD19" s="45"/>
       <c r="AH19" s="0"/>
-      <c r="AN19" s="149"/>
+      <c r="AN19" s="148"/>
       <c r="AO19" s="45"/>
       <c r="AP19" s="45"/>
-      <c r="AQ19" s="150"/>
+      <c r="AQ19" s="149"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="151" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="152"/>
+      <c r="A20" s="150" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="151"/>
       <c r="C20" s="50"/>
-      <c r="D20" s="152"/>
-      <c r="E20" s="152"/>
-      <c r="F20" s="152"/>
-      <c r="G20" s="152"/>
+      <c r="D20" s="151"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
       <c r="H20" s="50"/>
       <c r="I20" s="50"/>
-      <c r="J20" s="152"/>
-      <c r="K20" s="152"/>
-      <c r="L20" s="152"/>
+      <c r="J20" s="151"/>
+      <c r="K20" s="151"/>
+      <c r="L20" s="151"/>
       <c r="M20" s="50"/>
-      <c r="N20" s="153"/>
+      <c r="N20" s="152"/>
       <c r="O20" s="50"/>
-      <c r="P20" s="152" t="n">
+      <c r="P20" s="151" t="n">
         <v>0.001</v>
       </c>
       <c r="Q20" s="50"/>
@@ -3824,12 +3863,12 @@
         <v>2.79958631094939</v>
       </c>
       <c r="Y20" s="50"/>
-      <c r="Z20" s="136" t="n">
+      <c r="Z20" s="134" t="n">
         <f aca="false">2*PI()*(Q19/2)*P20</f>
         <v>0.000785398163397448</v>
       </c>
       <c r="AA20" s="50"/>
-      <c r="AB20" s="136" t="n">
+      <c r="AB20" s="134" t="n">
         <f aca="false">Z20+X20</f>
         <v>2.80037170911279</v>
       </c>
@@ -3844,41 +3883,41 @@
       <c r="AK20" s="50"/>
       <c r="AL20" s="50"/>
       <c r="AM20" s="50"/>
-      <c r="AN20" s="154"/>
+      <c r="AN20" s="153"/>
       <c r="AO20" s="50"/>
       <c r="AP20" s="50"/>
       <c r="AQ20" s="53"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="155" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="156"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="158"/>
-      <c r="I21" s="137"/>
-      <c r="J21" s="159"/>
-      <c r="K21" s="159"/>
-      <c r="L21" s="159"/>
-      <c r="M21" s="158"/>
-      <c r="N21" s="160"/>
-      <c r="O21" s="158"/>
-      <c r="P21" s="161" t="n">
+      <c r="A21" s="154" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="155"/>
+      <c r="C21" s="156"/>
+      <c r="D21" s="156"/>
+      <c r="E21" s="156"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="156"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="135"/>
+      <c r="J21" s="158"/>
+      <c r="K21" s="158"/>
+      <c r="L21" s="158"/>
+      <c r="M21" s="157"/>
+      <c r="N21" s="159"/>
+      <c r="O21" s="157"/>
+      <c r="P21" s="160" t="n">
         <v>1.35</v>
       </c>
-      <c r="Q21" s="162"/>
-      <c r="R21" s="163"/>
-      <c r="S21" s="163"/>
-      <c r="T21" s="137"/>
-      <c r="U21" s="158"/>
-      <c r="V21" s="158" t="n">
+      <c r="Q21" s="161"/>
+      <c r="R21" s="162"/>
+      <c r="S21" s="162"/>
+      <c r="T21" s="135"/>
+      <c r="U21" s="157"/>
+      <c r="V21" s="157" t="n">
         <v>0.944</v>
       </c>
-      <c r="W21" s="164" t="n">
+      <c r="W21" s="163" t="n">
         <f aca="false">0.944/2</f>
         <v>0.472</v>
       </c>
@@ -3886,116 +3925,116 @@
         <f aca="false">4*PI()*W21^2</f>
         <v>2.79958631094939</v>
       </c>
-      <c r="Y21" s="158"/>
-      <c r="Z21" s="136" t="n">
+      <c r="Y21" s="157"/>
+      <c r="Z21" s="134" t="n">
         <f aca="false">2*PI()*(Q19)*P21</f>
         <v>2.12057504117311</v>
       </c>
-      <c r="AA21" s="158"/>
-      <c r="AB21" s="136" t="n">
+      <c r="AA21" s="157"/>
+      <c r="AB21" s="134" t="n">
         <f aca="false">Z21+X21</f>
         <v>4.92016135212251</v>
       </c>
-      <c r="AC21" s="158"/>
-      <c r="AD21" s="158"/>
-      <c r="AE21" s="158"/>
-      <c r="AF21" s="158"/>
-      <c r="AG21" s="158"/>
-      <c r="AH21" s="158"/>
-      <c r="AI21" s="158"/>
-      <c r="AJ21" s="158"/>
-      <c r="AK21" s="158"/>
-      <c r="AL21" s="158"/>
-      <c r="AM21" s="158"/>
-      <c r="AN21" s="165"/>
-      <c r="AO21" s="158"/>
-      <c r="AP21" s="158"/>
-      <c r="AQ21" s="166"/>
+      <c r="AC21" s="157"/>
+      <c r="AD21" s="157"/>
+      <c r="AE21" s="157"/>
+      <c r="AF21" s="157"/>
+      <c r="AG21" s="157"/>
+      <c r="AH21" s="157"/>
+      <c r="AI21" s="157"/>
+      <c r="AJ21" s="157"/>
+      <c r="AK21" s="157"/>
+      <c r="AL21" s="157"/>
+      <c r="AM21" s="157"/>
+      <c r="AN21" s="164"/>
+      <c r="AO21" s="157"/>
+      <c r="AP21" s="157"/>
+      <c r="AQ21" s="165"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="167" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="168"/>
-      <c r="C22" s="169"/>
-      <c r="D22" s="170"/>
-      <c r="E22" s="141"/>
-      <c r="F22" s="141"/>
-      <c r="G22" s="141"/>
-      <c r="H22" s="141"/>
-      <c r="I22" s="141"/>
-      <c r="J22" s="141"/>
-      <c r="K22" s="141"/>
-      <c r="L22" s="141"/>
-      <c r="M22" s="141"/>
-      <c r="N22" s="141"/>
-      <c r="O22" s="141"/>
-      <c r="P22" s="141" t="n">
+      <c r="A22" s="166" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="167"/>
+      <c r="C22" s="168"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="140"/>
+      <c r="H22" s="140"/>
+      <c r="I22" s="140"/>
+      <c r="J22" s="140"/>
+      <c r="K22" s="140"/>
+      <c r="L22" s="140"/>
+      <c r="M22" s="140"/>
+      <c r="N22" s="140"/>
+      <c r="O22" s="140"/>
+      <c r="P22" s="140" t="n">
         <f aca="false">AVERAGE(P2:P14,P16:P17)</f>
         <v>0.82</v>
       </c>
-      <c r="Q22" s="141" t="n">
+      <c r="Q22" s="140" t="n">
         <f aca="false">AVERAGE(Q2:Q14,Q16:Q17)</f>
         <v>0.127733333333333</v>
       </c>
-      <c r="R22" s="171"/>
-      <c r="S22" s="141" t="n">
+      <c r="R22" s="170"/>
+      <c r="S22" s="140" t="n">
         <f aca="false">AVERAGE(S2:S14,S16:S17)</f>
         <v>0.0798327624786667</v>
       </c>
-      <c r="T22" s="141" t="n">
+      <c r="T22" s="140" t="n">
         <f aca="false">AVERAGE(T2:T14,T16:T17)</f>
         <v>0.06247913699</v>
       </c>
-      <c r="U22" s="141" t="n">
+      <c r="U22" s="140" t="n">
         <f aca="false">AVERAGE(U2:U14,U16:U17)</f>
         <v>0.0173536254886667</v>
       </c>
-      <c r="V22" s="141" t="n">
+      <c r="V22" s="140" t="n">
         <f aca="false">AVERAGE(V2:V14,V16:V17)</f>
         <v>0.471979217200875</v>
       </c>
-      <c r="W22" s="141" t="n">
+      <c r="W22" s="140" t="n">
         <f aca="false">AVERAGE(W2:W14,W16:W17)</f>
         <v>0.235989608600438</v>
       </c>
-      <c r="X22" s="141" t="n">
+      <c r="X22" s="171" t="n">
         <f aca="false">AVERAGE(X2:X14,X16:X17)</f>
         <v>0.731795066402826</v>
       </c>
-      <c r="Y22" s="141" t="n">
+      <c r="Y22" s="140" t="n">
         <f aca="false">AVERAGE(Y2:Y14,Y16:Y17)</f>
         <v>0.412352747612247</v>
       </c>
-      <c r="Z22" s="141" t="n">
+      <c r="Z22" s="140" t="n">
         <f aca="false">AVERAGE(Z2:Z14,Z16:Z17)</f>
         <v>0.318980353445178</v>
       </c>
-      <c r="AA22" s="141" t="n">
+      <c r="AA22" s="140" t="n">
         <f aca="false">AVERAGE(AA2:AA14,AA16:AA17)</f>
         <v>0.0108838737564887</v>
       </c>
-      <c r="AB22" s="141" t="n">
+      <c r="AB22" s="140" t="n">
         <f aca="false">AVERAGE(AB2:AB14,AB16:AB17)</f>
         <v>1.050775419848</v>
       </c>
-      <c r="AC22" s="80" t="n">
+      <c r="AC22" s="81" t="n">
         <v>1.08</v>
       </c>
-      <c r="AD22" s="141"/>
-      <c r="AE22" s="141"/>
-      <c r="AF22" s="141"/>
-      <c r="AG22" s="141"/>
-      <c r="AH22" s="141"/>
-      <c r="AI22" s="141"/>
-      <c r="AJ22" s="141"/>
-      <c r="AK22" s="141"/>
-      <c r="AL22" s="141"/>
-      <c r="AM22" s="141"/>
-      <c r="AN22" s="141"/>
-      <c r="AO22" s="141"/>
-      <c r="AP22" s="141"/>
-      <c r="AQ22" s="142"/>
+      <c r="AD22" s="140"/>
+      <c r="AE22" s="140"/>
+      <c r="AF22" s="140"/>
+      <c r="AG22" s="140"/>
+      <c r="AH22" s="140"/>
+      <c r="AI22" s="140"/>
+      <c r="AJ22" s="140"/>
+      <c r="AK22" s="140"/>
+      <c r="AL22" s="140"/>
+      <c r="AM22" s="140"/>
+      <c r="AN22" s="140"/>
+      <c r="AO22" s="140"/>
+      <c r="AP22" s="140"/>
+      <c r="AQ22" s="141"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="172"/>
@@ -4003,13 +4042,25 @@
       <c r="C23" s="173"/>
       <c r="D23" s="36"/>
       <c r="I23" s="0"/>
-      <c r="P23" s="148"/>
-      <c r="Q23" s="148"/>
-      <c r="R23" s="77" t="n">
+      <c r="P23" s="147"/>
+      <c r="Q23" s="147"/>
+      <c r="R23" s="78" t="n">
         <v>1</v>
       </c>
       <c r="S23" s="174"/>
       <c r="T23" s="174"/>
+      <c r="X23" s="131" t="n">
+        <f aca="false">4*PI()*W22^2</f>
+        <v>0.699834944306218</v>
+      </c>
+      <c r="Z23" s="44" t="n">
+        <f aca="false">2*PI()*(Q22/2)*P22</f>
+        <v>0.329054603327199</v>
+      </c>
+      <c r="AB23" s="134" t="n">
+        <f aca="false">Z23+X23</f>
+        <v>1.02888954763342</v>
+      </c>
       <c r="AD23" s="0"/>
       <c r="AE23" s="0"/>
       <c r="AF23" s="0"/>
@@ -4020,292 +4071,292 @@
       <c r="AQ23" s="45"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="69" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="70" t="n">
+      <c r="A24" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="71" t="n">
         <v>3</v>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>2</v>
-      </c>
-      <c r="D24" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="72" t="n">
+      <c r="C24" s="72" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="73" t="n">
         <v>1</v>
       </c>
-      <c r="F24" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="G24" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="H24" s="73" t="n">
+      <c r="F24" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" s="74" t="n">
         <v>32.6</v>
       </c>
-      <c r="I24" s="73" t="s">
+      <c r="I24" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="J24" s="74" t="n">
+      <c r="J24" s="75" t="n">
         <v>924.01</v>
       </c>
-      <c r="K24" s="74" t="n">
+      <c r="K24" s="75" t="n">
         <v>333.54</v>
       </c>
-      <c r="L24" s="74" t="n">
+      <c r="L24" s="75" t="n">
         <v>-257.4</v>
       </c>
-      <c r="M24" s="74" t="n">
+      <c r="M24" s="75" t="n">
         <v>0.114</v>
       </c>
-      <c r="N24" s="75" t="n">
+      <c r="N24" s="76" t="n">
         <v>199</v>
       </c>
-      <c r="O24" s="76" t="s">
-        <v>53</v>
-      </c>
-      <c r="P24" s="73" t="n">
+      <c r="O24" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="P24" s="74" t="n">
         <v>0.763</v>
       </c>
-      <c r="Q24" s="73" t="n">
+      <c r="Q24" s="74" t="n">
         <v>0.134</v>
       </c>
-      <c r="R24" s="77" t="n">
+      <c r="R24" s="78" t="n">
         <v>1</v>
       </c>
-      <c r="S24" s="73" t="n">
+      <c r="S24" s="74" t="n">
         <v>0.08501695029</v>
       </c>
-      <c r="T24" s="73" t="n">
+      <c r="T24" s="74" t="n">
         <v>0.0745871871</v>
       </c>
-      <c r="U24" s="73" t="n">
+      <c r="U24" s="74" t="n">
         <v>0.01042976319</v>
       </c>
-      <c r="V24" s="73"/>
-      <c r="W24" s="73"/>
-      <c r="X24" s="73"/>
-      <c r="Y24" s="73"/>
-      <c r="Z24" s="73"/>
-      <c r="AA24" s="73"/>
-      <c r="AB24" s="73"/>
-      <c r="AC24" s="80" t="n">
+      <c r="V24" s="74"/>
+      <c r="W24" s="74"/>
+      <c r="X24" s="74"/>
+      <c r="Y24" s="74"/>
+      <c r="Z24" s="74"/>
+      <c r="AA24" s="74"/>
+      <c r="AB24" s="134"/>
+      <c r="AC24" s="81" t="n">
         <v>1.08</v>
       </c>
-      <c r="AD24" s="81" t="n">
+      <c r="AD24" s="82" t="n">
         <v>1.85989007744307</v>
       </c>
-      <c r="AE24" s="81" t="n">
+      <c r="AE24" s="82" t="n">
         <v>0.324348142228853</v>
       </c>
       <c r="AF24" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="AG24" s="81" t="n">
+      <c r="AG24" s="82" t="n">
         <v>0.805034067065075</v>
       </c>
-      <c r="AH24" s="81" t="n">
+      <c r="AH24" s="82" t="n">
         <v>0.290119432876338</v>
       </c>
-      <c r="AI24" s="82" t="n">
+      <c r="AI24" s="83" t="n">
         <v>5</v>
       </c>
-      <c r="AJ24" s="82" t="n">
+      <c r="AJ24" s="83" t="n">
         <v>20</v>
       </c>
-      <c r="AK24" s="82" t="n">
+      <c r="AK24" s="83" t="n">
         <v>0.7</v>
       </c>
-      <c r="AL24" s="82" t="n">
+      <c r="AL24" s="83" t="n">
         <v>0.9</v>
       </c>
-      <c r="AM24" s="82" t="n">
+      <c r="AM24" s="83" t="n">
         <v>0.1</v>
       </c>
-      <c r="AN24" s="83" t="n">
+      <c r="AN24" s="84" t="n">
         <v>0.7</v>
       </c>
-      <c r="AO24" s="84" t="n">
+      <c r="AO24" s="85" t="n">
         <v>200</v>
       </c>
-      <c r="AP24" s="82" t="n">
+      <c r="AP24" s="83" t="n">
         <v>26</v>
       </c>
-      <c r="AQ24" s="85" t="n">
+      <c r="AQ24" s="86" t="n">
         <v>225</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="69" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="70" t="n">
+      <c r="A25" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="71" t="n">
         <v>3</v>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>2</v>
-      </c>
-      <c r="D25" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="72" t="n">
+      <c r="C25" s="72" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="73" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="H25" s="73" t="n">
+      <c r="F25" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" s="73" t="n">
+        <v>2</v>
+      </c>
+      <c r="H25" s="74" t="n">
         <v>50.6</v>
       </c>
-      <c r="I25" s="73" t="s">
+      <c r="I25" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="74" t="n">
+      <c r="J25" s="75" t="n">
         <v>873.38</v>
       </c>
-      <c r="K25" s="74" t="n">
+      <c r="K25" s="75" t="n">
         <v>331.97</v>
       </c>
-      <c r="L25" s="74" t="n">
+      <c r="L25" s="75" t="n">
         <v>-289.32</v>
       </c>
-      <c r="M25" s="74" t="n">
+      <c r="M25" s="75" t="n">
         <v>0.039</v>
       </c>
-      <c r="N25" s="75" t="n">
+      <c r="N25" s="76" t="n">
         <v>3806</v>
       </c>
-      <c r="O25" s="76" t="s">
-        <v>55</v>
-      </c>
-      <c r="P25" s="73" t="n">
+      <c r="O25" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="P25" s="74" t="n">
         <v>0.905</v>
       </c>
-      <c r="Q25" s="73" t="n">
+      <c r="Q25" s="74" t="n">
         <v>0.085</v>
       </c>
-      <c r="R25" s="94" t="n">
+      <c r="R25" s="95" t="n">
         <v>11</v>
       </c>
-      <c r="S25" s="73" t="n">
+      <c r="S25" s="74" t="n">
         <v>0.0783942101</v>
       </c>
-      <c r="T25" s="73" t="n">
+      <c r="T25" s="74" t="n">
         <v>0.06459193692</v>
       </c>
-      <c r="U25" s="73" t="n">
+      <c r="U25" s="74" t="n">
         <v>0.01380227318</v>
       </c>
-      <c r="V25" s="73"/>
-      <c r="W25" s="73"/>
-      <c r="X25" s="73"/>
-      <c r="Y25" s="73"/>
-      <c r="Z25" s="73"/>
-      <c r="AA25" s="73"/>
-      <c r="AB25" s="73"/>
-      <c r="AC25" s="80" t="n">
+      <c r="V25" s="74"/>
+      <c r="W25" s="74"/>
+      <c r="X25" s="74"/>
+      <c r="Y25" s="74"/>
+      <c r="Z25" s="74"/>
+      <c r="AA25" s="74"/>
+      <c r="AB25" s="74"/>
+      <c r="AC25" s="81" t="n">
         <v>1.08</v>
       </c>
-      <c r="AD25" s="82" t="n">
+      <c r="AD25" s="83" t="n">
         <v>1.85989007744307</v>
       </c>
-      <c r="AE25" s="85" t="n">
+      <c r="AE25" s="86" t="n">
         <v>0.324348142228853</v>
       </c>
-      <c r="AF25" s="82" t="n">
+      <c r="AF25" s="83" t="n">
         <v>8</v>
       </c>
-      <c r="AG25" s="82" t="n">
+      <c r="AG25" s="83" t="n">
         <v>0.805034067065075</v>
       </c>
-      <c r="AH25" s="82" t="n">
+      <c r="AH25" s="83" t="n">
         <v>0.290119432876338</v>
       </c>
-      <c r="AI25" s="82"/>
-      <c r="AJ25" s="82"/>
-      <c r="AK25" s="82"/>
-      <c r="AL25" s="82"/>
-      <c r="AM25" s="82"/>
-      <c r="AN25" s="83"/>
-      <c r="AO25" s="84"/>
-      <c r="AP25" s="82"/>
-      <c r="AQ25" s="85"/>
+      <c r="AI25" s="83"/>
+      <c r="AJ25" s="83"/>
+      <c r="AK25" s="83"/>
+      <c r="AL25" s="83"/>
+      <c r="AM25" s="83"/>
+      <c r="AN25" s="84"/>
+      <c r="AO25" s="85"/>
+      <c r="AP25" s="83"/>
+      <c r="AQ25" s="86"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="90" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="91" t="n">
+      <c r="A26" s="91" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="92" t="n">
         <v>4</v>
       </c>
-      <c r="C26" s="92" t="n">
+      <c r="C26" s="93" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="93" t="n">
+      <c r="D26" s="94" t="n">
         <v>91</v>
       </c>
-      <c r="E26" s="93" t="n">
-        <v>2</v>
-      </c>
-      <c r="F26" s="93" t="n">
+      <c r="E26" s="94" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" s="94" t="n">
         <v>1</v>
       </c>
-      <c r="G26" s="93" t="n">
+      <c r="G26" s="94" t="n">
         <v>1</v>
       </c>
-      <c r="H26" s="94" t="n">
+      <c r="H26" s="95" t="n">
         <v>83.8</v>
       </c>
-      <c r="I26" s="94" t="s">
+      <c r="I26" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="J26" s="95" t="n">
+      <c r="J26" s="96" t="n">
         <v>-5.56</v>
       </c>
-      <c r="K26" s="95" t="n">
+      <c r="K26" s="96" t="n">
         <v>-325.88</v>
       </c>
-      <c r="L26" s="96" t="n">
+      <c r="L26" s="97" t="n">
         <v>-451.42</v>
       </c>
-      <c r="M26" s="97" t="n">
+      <c r="M26" s="98" t="n">
         <v>0.14</v>
       </c>
-      <c r="N26" s="98" t="n">
+      <c r="N26" s="99" t="n">
         <v>82</v>
       </c>
-      <c r="O26" s="99"/>
-      <c r="P26" s="94" t="n">
+      <c r="O26" s="175"/>
+      <c r="P26" s="95" t="n">
         <v>0.782</v>
       </c>
-      <c r="Q26" s="94" t="n">
+      <c r="Q26" s="95" t="n">
         <v>0.164</v>
       </c>
       <c r="R26" s="111" t="n">
         <v>15</v>
       </c>
-      <c r="S26" s="94" t="n">
+      <c r="S26" s="95" t="n">
         <v>0.16884774101</v>
       </c>
-      <c r="T26" s="94" t="n">
+      <c r="T26" s="95" t="n">
         <v>0.13906972096</v>
       </c>
-      <c r="U26" s="94" t="n">
+      <c r="U26" s="95" t="n">
         <v>0.02977802005</v>
       </c>
-      <c r="V26" s="94"/>
-      <c r="W26" s="94"/>
-      <c r="X26" s="94"/>
-      <c r="Y26" s="94"/>
-      <c r="Z26" s="94"/>
-      <c r="AA26" s="94"/>
-      <c r="AB26" s="94"/>
+      <c r="V26" s="95"/>
+      <c r="W26" s="95"/>
+      <c r="X26" s="95"/>
+      <c r="Y26" s="95"/>
+      <c r="Z26" s="95"/>
+      <c r="AA26" s="95"/>
+      <c r="AB26" s="95"/>
       <c r="AC26" s="0"/>
-      <c r="AD26" s="94" t="n">
+      <c r="AD26" s="95" t="n">
         <v>1.26083037757995</v>
       </c>
       <c r="AE26" s="102" t="n">
@@ -4341,7 +4392,7 @@
       <c r="AO26" s="105" t="n">
         <v>275</v>
       </c>
-      <c r="AP26" s="94" t="n">
+      <c r="AP26" s="95" t="n">
         <v>176</v>
       </c>
       <c r="AQ26" s="102" t="n">
@@ -4350,7 +4401,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="107" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B27" s="108" t="n">
         <v>4</v>
@@ -4392,7 +4443,7 @@
         <v>4358</v>
       </c>
       <c r="O27" s="114" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P27" s="111" t="n">
         <v>1.266</v>
@@ -4419,7 +4470,7 @@
       <c r="Z27" s="111"/>
       <c r="AA27" s="111"/>
       <c r="AB27" s="111"/>
-      <c r="AC27" s="80" t="n">
+      <c r="AC27" s="81" t="n">
         <v>1.08</v>
       </c>
       <c r="AD27" s="117" t="n">
@@ -4467,7 +4518,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="107" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B28" s="108" t="n">
         <v>4</v>
@@ -4509,7 +4560,7 @@
         <v>3923</v>
       </c>
       <c r="O28" s="114" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="P28" s="111" t="n">
         <v>1.121</v>
@@ -4517,7 +4568,7 @@
       <c r="Q28" s="111" t="n">
         <v>0.102</v>
       </c>
-      <c r="R28" s="171"/>
+      <c r="R28" s="170"/>
       <c r="S28" s="111" t="n">
         <v>0.02865474235</v>
       </c>
@@ -4534,7 +4585,7 @@
       <c r="Z28" s="111"/>
       <c r="AA28" s="111"/>
       <c r="AB28" s="111"/>
-      <c r="AC28" s="80" t="n">
+      <c r="AC28" s="81" t="n">
         <v>1.08</v>
       </c>
       <c r="AD28" s="117" t="n">
@@ -4664,7 +4715,7 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I35" s="0"/>
       <c r="AE35" s="45"/>
-      <c r="AF35" s="175"/>
+      <c r="AF35" s="176"/>
       <c r="AG35" s="45"/>
       <c r="AH35" s="45"/>
       <c r="AI35" s="45"/>
@@ -4677,7 +4728,7 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I36" s="0"/>
       <c r="AE36" s="45"/>
-      <c r="AF36" s="175"/>
+      <c r="AF36" s="176"/>
       <c r="AG36" s="45"/>
       <c r="AH36" s="45"/>
       <c r="AI36" s="45"/>

</xml_diff>

<commit_message>
corretc the short pulse to be unsplit between pre-post syn
</commit_message>
<xml_diff>
--- a/cells_initial_information/Data2.xlsx
+++ b/cells_initial_information/Data2.xlsx
@@ -291,6 +291,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -312,6 +313,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -319,12 +321,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -332,6 +336,7 @@
       <color rgb="FF81D41A"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -339,6 +344,7 @@
       <color rgb="FFFF972F"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -346,6 +352,7 @@
       <color rgb="FFFFA6A6"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -353,18 +360,21 @@
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -372,6 +382,7 @@
       <color rgb="FF729FCF"/>
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -379,18 +390,21 @@
       <color rgb="FF729FCF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF729FCF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -398,12 +412,14 @@
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -411,6 +427,7 @@
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1511,8 +1528,8 @@
   </sheetPr>
   <dimension ref="A1:BF41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q45" activeCellId="0" sqref="Q45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1959,10 +1976,10 @@
         <v>120</v>
       </c>
       <c r="E4" s="45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="45" t="n">
         <v>1</v>
@@ -2095,10 +2112,10 @@
         <v>202</v>
       </c>
       <c r="E5" s="45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="45" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
correct a wird mistake
</commit_message>
<xml_diff>
--- a/cells_initial_information/Data2.xlsx
+++ b/cells_initial_information/Data2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
   <si>
     <t xml:space="preserve">cell_name</t>
   </si>
@@ -223,9 +223,6 @@
     <t xml:space="preserve">2017_04_03_B</t>
   </si>
   <si>
-    <t xml:space="preserve">552,59</t>
-  </si>
-  <si>
     <t xml:space="preserve">(-606.35; 503.26; -222.56)</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
   </si>
   <si>
     <t xml:space="preserve">c69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-302.68'file:///ems/elsc-labs/segev-i/moria.fridman/project/analysis_groger_cells/cells_outputs_data_short/synaptic_location_seperate_test.xlsx'#$Sheet1.E2</t>
   </si>
   <si>
     <t xml:space="preserve">(76.95; 1865.80; -250.50)</t>
@@ -306,7 +300,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -328,14 +321,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF999999"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -343,14 +334,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -358,7 +347,6 @@
       <color rgb="FF81D41A"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -366,7 +354,6 @@
       <color rgb="FFFF972F"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -374,7 +361,6 @@
       <color rgb="FFFFA6A6"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -382,21 +368,18 @@
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -404,7 +387,6 @@
       <color rgb="FF729FCF"/>
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -412,21 +394,18 @@
       <color rgb="FF729FCF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF729FCF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -434,14 +413,12 @@
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -449,7 +426,6 @@
       <color rgb="FF999999"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -457,7 +433,6 @@
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1606,8 +1581,8 @@
   </sheetPr>
   <dimension ref="A1:BI41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3075,8 +3050,8 @@
       <c r="J11" s="50" t="n">
         <v>-666.98</v>
       </c>
-      <c r="K11" s="50" t="s">
-        <v>67</v>
+      <c r="K11" s="50" t="n">
+        <v>552.59</v>
       </c>
       <c r="L11" s="50" t="n">
         <v>-244.82</v>
@@ -3097,7 +3072,7 @@
         <v>4746</v>
       </c>
       <c r="R11" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S11" s="49" t="n">
         <v>0.823</v>
@@ -3191,7 +3166,7 @@
     </row>
     <row r="12" s="104" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="89" t="n">
         <v>4</v>
@@ -3242,7 +3217,7 @@
         <v>82</v>
       </c>
       <c r="R12" s="97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S12" s="92" t="n">
         <v>0.782</v>
@@ -3351,7 +3326,7 @@
     </row>
     <row r="13" s="117" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="105" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="106" t="n">
         <v>4</v>
@@ -3402,7 +3377,7 @@
         <v>4358</v>
       </c>
       <c r="R13" s="110" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S13" s="109" t="n">
         <v>1.266</v>
@@ -3513,7 +3488,7 @@
     </row>
     <row r="14" s="117" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="105" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="106" t="n">
         <v>4</v>
@@ -3564,7 +3539,7 @@
         <v>3923</v>
       </c>
       <c r="R14" s="110" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S14" s="109" t="n">
         <v>1.121</v>
@@ -3657,7 +3632,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="118" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>5</v>
@@ -3666,7 +3641,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="119" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="119" t="n">
         <v>1</v>
@@ -3708,7 +3683,7 @@
         <v>17004</v>
       </c>
       <c r="R15" s="38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S15" s="37" t="n">
         <v>0</v>
@@ -3802,7 +3777,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="122" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>5</v>
@@ -3811,7 +3786,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="119" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E16" s="119" t="n">
         <v>1</v>
@@ -3834,8 +3809,8 @@
       <c r="K16" s="38" t="n">
         <v>2255.16</v>
       </c>
-      <c r="L16" s="38" t="s">
-        <v>78</v>
+      <c r="L16" s="38" t="n">
+        <v>-302.68</v>
       </c>
       <c r="M16" s="39" t="n">
         <v>76.95</v>
@@ -3853,7 +3828,7 @@
         <v>17261</v>
       </c>
       <c r="R16" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S16" s="37" t="n">
         <v>0.806</v>
@@ -3919,7 +3894,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="123" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" s="124" t="n">
         <v>1</v>
@@ -3928,7 +3903,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="126" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E17" s="126" t="n">
         <v>2</v>
@@ -3970,7 +3945,7 @@
         <v>5478</v>
       </c>
       <c r="R17" s="128" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="S17" s="127" t="n">
         <v>1.063</v>
@@ -4115,7 +4090,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="140" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" s="141"/>
       <c r="C19" s="24"/>
@@ -4167,7 +4142,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="149" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" s="150"/>
       <c r="C20" s="49"/>
@@ -4233,7 +4208,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="154" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" s="155"/>
       <c r="C21" s="156"/>
@@ -4299,7 +4274,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="167" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" s="168"/>
       <c r="C22" s="169"/>
@@ -4424,7 +4399,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="68" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B24" s="69" t="n">
         <v>3</v>
@@ -4550,7 +4525,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="68" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" s="69" t="n">
         <v>3</v>
@@ -4658,7 +4633,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="88" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B26" s="89" t="n">
         <v>4</v>
@@ -4780,7 +4755,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="105" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="106" t="n">
         <v>4</v>
@@ -4831,7 +4806,7 @@
         <v>4358</v>
       </c>
       <c r="R27" s="181" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S27" s="109" t="n">
         <v>1.266</v>
@@ -4906,7 +4881,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="105" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28" s="106" t="n">
         <v>4</v>
@@ -4957,7 +4932,7 @@
         <v>3923</v>
       </c>
       <c r="R28" s="181" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S28" s="109" t="n">
         <v>1.121</v>

</xml_diff>